<commit_message>
gantt chart having all details
</commit_message>
<xml_diff>
--- a/gantt-chart-Alpha-cab.xlsx
+++ b/gantt-chart-Alpha-cab.xlsx
@@ -16,7 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="prevWBS" localSheetId="0">GanttChart!$A1048576</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$1:$BN$39</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$1:$BO$39</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">GanttChart!$4:$7</definedName>
     <definedName name="valuevx">42.314159</definedName>
     <definedName name="vertex42_copyright" hidden="1">"© 2006-2018 Vertex42 LLC"</definedName>
@@ -143,7 +143,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E7" authorId="0" shapeId="0">
+    <comment ref="F7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -266,7 +266,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F7" authorId="1" shapeId="0">
+    <comment ref="G7" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -290,7 +290,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G7" authorId="0" shapeId="0">
+    <comment ref="H7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -372,7 +372,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H7" authorId="0" shapeId="0">
+    <comment ref="I7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -396,7 +396,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I7" authorId="0" shapeId="0">
+    <comment ref="J7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -425,7 +425,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="53">
   <si>
     <t>WBS</t>
   </si>
@@ -522,9 +522,6 @@
     <t>Ameera</t>
   </si>
   <si>
-    <t xml:space="preserve">make sessions for users </t>
-  </si>
-  <si>
     <t>Implementation of a complete database</t>
   </si>
   <si>
@@ -535,9 +532,6 @@
   </si>
   <si>
     <t>Display list of all registered users (driver/customer)</t>
-  </si>
-  <si>
-    <t>Add drivers in the drivers list</t>
   </si>
   <si>
     <t>Book a taxi by date and time</t>
@@ -556,12 +550,6 @@
   </si>
   <si>
     <t>Delete driver</t>
-  </si>
-  <si>
-    <t>Update destination’s price(web service )</t>
-  </si>
-  <si>
-    <t>List customers served per day (destination+ fee)</t>
   </si>
   <si>
     <t>Authentication</t>
@@ -595,6 +583,27 @@
   </si>
   <si>
     <t xml:space="preserve">customer invoice </t>
+  </si>
+  <si>
+    <t>WORKED</t>
+  </si>
+  <si>
+    <t>Everyone</t>
+  </si>
+  <si>
+    <t>make sessions for admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Bookings List</t>
+  </si>
+  <si>
+    <t>Update price</t>
+  </si>
+  <si>
+    <t>Add user</t>
   </si>
 </sst>
 </file>
@@ -1579,22 +1588,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="35" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="35" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="33" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="9" fontId="35" fillId="23" borderId="0" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="33" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1604,26 +1613,26 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="35" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="33" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="35" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="35" fillId="23" borderId="0" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="33" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1673,7 +1682,21 @@
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1812,21 +1835,21 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$4" horiz="1" max="100" min="1" page="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$I$4" horiz="1" max="100" min="1" page="0" val="12"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>781050</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>309033</xdr:rowOff>
     </xdr:to>
@@ -1835,7 +1858,7 @@
         <xdr:cNvPr id="8236" name="Text Box 44" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C200000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002C200000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1880,13 +1903,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>9</xdr:col>
+          <xdr:col>10</xdr:col>
           <xdr:colOff>95250</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>123825</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>27</xdr:col>
+          <xdr:col>28</xdr:col>
           <xdr:colOff>114300</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
@@ -1899,7 +1922,7 @@
                   <a14:compatExt spid="_x0000_s8238"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002E200000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002E200000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2219,11 +2242,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BN49"/>
+  <dimension ref="A1:BV49"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I32" sqref="I32"/>
+      <pane ySplit="7" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2232,29 +2255,36 @@
     <col min="2" max="2" width="19" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="6.85546875" style="6" hidden="1" customWidth="1"/>
-    <col min="5" max="6" width="12" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="1.85546875" style="1" customWidth="1"/>
-    <col min="11" max="66" width="2.42578125" style="1" customWidth="1"/>
-    <col min="67" max="16384" width="9.140625" style="3"/>
+    <col min="5" max="5" width="10.140625" style="6" customWidth="1"/>
+    <col min="6" max="7" width="12" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="1.85546875" style="1" customWidth="1"/>
+    <col min="12" max="67" width="2.42578125" style="1" customWidth="1"/>
+    <col min="68" max="68" width="3.28515625" style="3" customWidth="1"/>
+    <col min="69" max="69" width="2.7109375" style="3" customWidth="1"/>
+    <col min="70" max="71" width="3.140625" style="3" customWidth="1"/>
+    <col min="72" max="72" width="3" style="3" customWidth="1"/>
+    <col min="73" max="73" width="4" style="3" customWidth="1"/>
+    <col min="74" max="74" width="4.42578125" style="3" customWidth="1"/>
+    <col min="75" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:74" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="79" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
-      <c r="I1" s="83"/>
-      <c r="K1" s="94" t="s">
+      <c r="G1" s="14"/>
+      <c r="J1" s="83"/>
+      <c r="L1" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="94"/>
       <c r="M1" s="94"/>
       <c r="N1" s="94"/>
       <c r="O1" s="94"/>
@@ -2274,19 +2304,21 @@
       <c r="AC1" s="94"/>
       <c r="AD1" s="94"/>
       <c r="AE1" s="94"/>
+      <c r="AF1" s="94"/>
     </row>
-    <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:74" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
       <c r="D2" s="13"/>
-      <c r="E2" s="84"/>
+      <c r="E2" s="13"/>
       <c r="F2" s="84"/>
-      <c r="H2" s="2"/>
+      <c r="G2" s="84"/>
+      <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:66" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:74" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="19"/>
       <c r="B3" s="15"/>
       <c r="C3" s="4"/>
@@ -2294,8 +2326,8 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
-      <c r="H3" s="2"/>
-      <c r="K3" s="9"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="2"/>
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
       <c r="N3" s="9"/>
@@ -2312,108 +2344,122 @@
       <c r="Y3" s="9"/>
       <c r="Z3" s="9"/>
       <c r="AA3" s="9"/>
+      <c r="AB3" s="9"/>
     </row>
-    <row r="4" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="64"/>
+    <row r="4" spans="1:74" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="64" t="s">
+        <v>49</v>
+      </c>
       <c r="B4" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="96">
+      <c r="C4" s="99">
         <v>43884</v>
       </c>
-      <c r="D4" s="96"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="68" t="s">
+      <c r="D4" s="99"/>
+      <c r="E4" s="99"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="82">
-        <v>1</v>
-      </c>
-      <c r="I4" s="66"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="88" t="str">
-        <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 1</v>
-      </c>
-      <c r="L4" s="89"/>
-      <c r="M4" s="89"/>
-      <c r="N4" s="89"/>
-      <c r="O4" s="89"/>
-      <c r="P4" s="89"/>
-      <c r="Q4" s="90"/>
-      <c r="R4" s="88" t="str">
-        <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 2</v>
-      </c>
-      <c r="S4" s="89"/>
-      <c r="T4" s="89"/>
-      <c r="U4" s="89"/>
-      <c r="V4" s="89"/>
-      <c r="W4" s="89"/>
-      <c r="X4" s="90"/>
-      <c r="Y4" s="88" t="str">
-        <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 3</v>
-      </c>
-      <c r="Z4" s="89"/>
-      <c r="AA4" s="89"/>
-      <c r="AB4" s="89"/>
-      <c r="AC4" s="89"/>
-      <c r="AD4" s="89"/>
-      <c r="AE4" s="90"/>
-      <c r="AF4" s="88" t="str">
-        <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 4</v>
-      </c>
-      <c r="AG4" s="89"/>
-      <c r="AH4" s="89"/>
-      <c r="AI4" s="89"/>
-      <c r="AJ4" s="89"/>
-      <c r="AK4" s="89"/>
-      <c r="AL4" s="90"/>
-      <c r="AM4" s="88" t="str">
-        <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 5</v>
-      </c>
-      <c r="AN4" s="89"/>
-      <c r="AO4" s="89"/>
-      <c r="AP4" s="89"/>
-      <c r="AQ4" s="89"/>
-      <c r="AR4" s="89"/>
-      <c r="AS4" s="90"/>
-      <c r="AT4" s="88" t="str">
-        <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 6</v>
-      </c>
-      <c r="AU4" s="89"/>
-      <c r="AV4" s="89"/>
-      <c r="AW4" s="89"/>
-      <c r="AX4" s="89"/>
-      <c r="AY4" s="89"/>
-      <c r="AZ4" s="90"/>
-      <c r="BA4" s="88" t="str">
-        <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 7</v>
-      </c>
-      <c r="BB4" s="89"/>
-      <c r="BC4" s="89"/>
-      <c r="BD4" s="89"/>
-      <c r="BE4" s="89"/>
-      <c r="BF4" s="89"/>
-      <c r="BG4" s="90"/>
-      <c r="BH4" s="88" t="str">
-        <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 8</v>
-      </c>
-      <c r="BI4" s="89"/>
-      <c r="BJ4" s="89"/>
-      <c r="BK4" s="89"/>
-      <c r="BL4" s="89"/>
-      <c r="BM4" s="89"/>
-      <c r="BN4" s="90"/>
+      <c r="I4" s="82">
+        <v>12</v>
+      </c>
+      <c r="J4" s="66"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="96" t="str">
+        <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 12</v>
+      </c>
+      <c r="M4" s="97"/>
+      <c r="N4" s="97"/>
+      <c r="O4" s="97"/>
+      <c r="P4" s="97"/>
+      <c r="Q4" s="97"/>
+      <c r="R4" s="98"/>
+      <c r="S4" s="96" t="str">
+        <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 13</v>
+      </c>
+      <c r="T4" s="97"/>
+      <c r="U4" s="97"/>
+      <c r="V4" s="97"/>
+      <c r="W4" s="97"/>
+      <c r="X4" s="97"/>
+      <c r="Y4" s="98"/>
+      <c r="Z4" s="96" t="str">
+        <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 14</v>
+      </c>
+      <c r="AA4" s="97"/>
+      <c r="AB4" s="97"/>
+      <c r="AC4" s="97"/>
+      <c r="AD4" s="97"/>
+      <c r="AE4" s="97"/>
+      <c r="AF4" s="98"/>
+      <c r="AG4" s="96" t="str">
+        <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 15</v>
+      </c>
+      <c r="AH4" s="97"/>
+      <c r="AI4" s="97"/>
+      <c r="AJ4" s="97"/>
+      <c r="AK4" s="97"/>
+      <c r="AL4" s="97"/>
+      <c r="AM4" s="98"/>
+      <c r="AN4" s="96" t="str">
+        <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 16</v>
+      </c>
+      <c r="AO4" s="97"/>
+      <c r="AP4" s="97"/>
+      <c r="AQ4" s="97"/>
+      <c r="AR4" s="97"/>
+      <c r="AS4" s="97"/>
+      <c r="AT4" s="98"/>
+      <c r="AU4" s="96" t="str">
+        <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 17</v>
+      </c>
+      <c r="AV4" s="97"/>
+      <c r="AW4" s="97"/>
+      <c r="AX4" s="97"/>
+      <c r="AY4" s="97"/>
+      <c r="AZ4" s="97"/>
+      <c r="BA4" s="98"/>
+      <c r="BB4" s="96" t="str">
+        <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 18</v>
+      </c>
+      <c r="BC4" s="97"/>
+      <c r="BD4" s="97"/>
+      <c r="BE4" s="97"/>
+      <c r="BF4" s="97"/>
+      <c r="BG4" s="97"/>
+      <c r="BH4" s="98"/>
+      <c r="BI4" s="96" t="str">
+        <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 19</v>
+      </c>
+      <c r="BJ4" s="97"/>
+      <c r="BK4" s="97"/>
+      <c r="BL4" s="97"/>
+      <c r="BM4" s="97"/>
+      <c r="BN4" s="97"/>
+      <c r="BO4" s="98"/>
+      <c r="BP4" s="96" t="str">
+        <f>"Week "&amp;(BP6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 20</v>
+      </c>
+      <c r="BQ4" s="97"/>
+      <c r="BR4" s="97"/>
+      <c r="BS4" s="97"/>
+      <c r="BT4" s="97"/>
+      <c r="BU4" s="97"/>
+      <c r="BV4" s="98"/>
     </row>
-    <row r="5" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:74" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="64"/>
       <c r="B5" s="68" t="s">
         <v>11</v>
@@ -2423,329 +2469,369 @@
       </c>
       <c r="D5" s="95"/>
       <c r="E5" s="95"/>
-      <c r="F5" s="67"/>
+      <c r="F5" s="95"/>
       <c r="G5" s="67"/>
       <c r="H5" s="67"/>
       <c r="I5" s="67"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="91">
-        <f>K6</f>
-        <v>43885</v>
-      </c>
-      <c r="L5" s="92"/>
-      <c r="M5" s="92"/>
-      <c r="N5" s="92"/>
-      <c r="O5" s="92"/>
-      <c r="P5" s="92"/>
-      <c r="Q5" s="93"/>
-      <c r="R5" s="91">
-        <f>R6</f>
-        <v>43892</v>
-      </c>
-      <c r="S5" s="92"/>
-      <c r="T5" s="92"/>
-      <c r="U5" s="92"/>
-      <c r="V5" s="92"/>
-      <c r="W5" s="92"/>
-      <c r="X5" s="93"/>
-      <c r="Y5" s="91">
-        <f>Y6</f>
-        <v>43899</v>
-      </c>
-      <c r="Z5" s="92"/>
-      <c r="AA5" s="92"/>
-      <c r="AB5" s="92"/>
-      <c r="AC5" s="92"/>
-      <c r="AD5" s="92"/>
-      <c r="AE5" s="93"/>
-      <c r="AF5" s="91">
-        <f>AF6</f>
-        <v>43906</v>
-      </c>
-      <c r="AG5" s="92"/>
-      <c r="AH5" s="92"/>
-      <c r="AI5" s="92"/>
-      <c r="AJ5" s="92"/>
-      <c r="AK5" s="92"/>
-      <c r="AL5" s="93"/>
-      <c r="AM5" s="91">
-        <f>AM6</f>
-        <v>43913</v>
-      </c>
-      <c r="AN5" s="92"/>
-      <c r="AO5" s="92"/>
-      <c r="AP5" s="92"/>
-      <c r="AQ5" s="92"/>
-      <c r="AR5" s="92"/>
-      <c r="AS5" s="93"/>
-      <c r="AT5" s="91">
-        <f>AT6</f>
-        <v>43920</v>
-      </c>
-      <c r="AU5" s="92"/>
-      <c r="AV5" s="92"/>
-      <c r="AW5" s="92"/>
-      <c r="AX5" s="92"/>
-      <c r="AY5" s="92"/>
-      <c r="AZ5" s="93"/>
-      <c r="BA5" s="91">
-        <f>BA6</f>
-        <v>43927</v>
-      </c>
-      <c r="BB5" s="92"/>
-      <c r="BC5" s="92"/>
-      <c r="BD5" s="92"/>
-      <c r="BE5" s="92"/>
-      <c r="BF5" s="92"/>
-      <c r="BG5" s="93"/>
-      <c r="BH5" s="91">
-        <f>BH6</f>
-        <v>43934</v>
-      </c>
-      <c r="BI5" s="92"/>
-      <c r="BJ5" s="92"/>
-      <c r="BK5" s="92"/>
-      <c r="BL5" s="92"/>
-      <c r="BM5" s="92"/>
-      <c r="BN5" s="93"/>
+      <c r="J5" s="67"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="100">
+        <f>L6</f>
+        <v>43962</v>
+      </c>
+      <c r="M5" s="101"/>
+      <c r="N5" s="101"/>
+      <c r="O5" s="101"/>
+      <c r="P5" s="101"/>
+      <c r="Q5" s="101"/>
+      <c r="R5" s="102"/>
+      <c r="S5" s="100">
+        <f>S6</f>
+        <v>43969</v>
+      </c>
+      <c r="T5" s="101"/>
+      <c r="U5" s="101"/>
+      <c r="V5" s="101"/>
+      <c r="W5" s="101"/>
+      <c r="X5" s="101"/>
+      <c r="Y5" s="102"/>
+      <c r="Z5" s="100">
+        <f>Z6</f>
+        <v>43976</v>
+      </c>
+      <c r="AA5" s="101"/>
+      <c r="AB5" s="101"/>
+      <c r="AC5" s="101"/>
+      <c r="AD5" s="101"/>
+      <c r="AE5" s="101"/>
+      <c r="AF5" s="102"/>
+      <c r="AG5" s="100">
+        <f>AG6</f>
+        <v>43983</v>
+      </c>
+      <c r="AH5" s="101"/>
+      <c r="AI5" s="101"/>
+      <c r="AJ5" s="101"/>
+      <c r="AK5" s="101"/>
+      <c r="AL5" s="101"/>
+      <c r="AM5" s="102"/>
+      <c r="AN5" s="100">
+        <f>AN6</f>
+        <v>43990</v>
+      </c>
+      <c r="AO5" s="101"/>
+      <c r="AP5" s="101"/>
+      <c r="AQ5" s="101"/>
+      <c r="AR5" s="101"/>
+      <c r="AS5" s="101"/>
+      <c r="AT5" s="102"/>
+      <c r="AU5" s="100">
+        <f>AU6</f>
+        <v>43997</v>
+      </c>
+      <c r="AV5" s="101"/>
+      <c r="AW5" s="101"/>
+      <c r="AX5" s="101"/>
+      <c r="AY5" s="101"/>
+      <c r="AZ5" s="101"/>
+      <c r="BA5" s="102"/>
+      <c r="BB5" s="100">
+        <f>BB6</f>
+        <v>44004</v>
+      </c>
+      <c r="BC5" s="101"/>
+      <c r="BD5" s="101"/>
+      <c r="BE5" s="101"/>
+      <c r="BF5" s="101"/>
+      <c r="BG5" s="101"/>
+      <c r="BH5" s="102"/>
+      <c r="BI5" s="100">
+        <f>BI6</f>
+        <v>44011</v>
+      </c>
+      <c r="BJ5" s="101"/>
+      <c r="BK5" s="101"/>
+      <c r="BL5" s="101"/>
+      <c r="BM5" s="101"/>
+      <c r="BN5" s="101"/>
+      <c r="BO5" s="102"/>
+      <c r="BP5" s="100">
+        <f>BP6</f>
+        <v>44018</v>
+      </c>
+      <c r="BQ5" s="101"/>
+      <c r="BR5" s="101"/>
+      <c r="BS5" s="101"/>
+      <c r="BT5" s="101"/>
+      <c r="BU5" s="101"/>
+      <c r="BV5" s="102"/>
     </row>
-    <row r="6" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A6" s="16"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
       <c r="D6" s="18"/>
-      <c r="E6" s="17"/>
+      <c r="E6" s="18"/>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
       <c r="H6" s="17"/>
       <c r="I6" s="17"/>
       <c r="J6" s="17"/>
-      <c r="K6" s="48">
-        <f>C4-WEEKDAY(C4,1)+2+7*(H4-1)</f>
-        <v>43885</v>
-      </c>
-      <c r="L6" s="39">
-        <f t="shared" ref="L6:AQ6" si="0">K6+1</f>
-        <v>43886</v>
+      <c r="K6" s="17"/>
+      <c r="L6" s="48">
+        <f>C4-WEEKDAY(C4,1)+2+7*(I4-1)</f>
+        <v>43962</v>
       </c>
       <c r="M6" s="39">
-        <f t="shared" si="0"/>
-        <v>43887</v>
+        <f t="shared" ref="M6:AR6" si="0">L6+1</f>
+        <v>43963</v>
       </c>
       <c r="N6" s="39">
         <f t="shared" si="0"/>
-        <v>43888</v>
+        <v>43964</v>
       </c>
       <c r="O6" s="39">
         <f t="shared" si="0"/>
-        <v>43889</v>
+        <v>43965</v>
       </c>
       <c r="P6" s="39">
         <f t="shared" si="0"/>
-        <v>43890</v>
-      </c>
-      <c r="Q6" s="49">
+        <v>43966</v>
+      </c>
+      <c r="Q6" s="39">
         <f t="shared" si="0"/>
-        <v>43891</v>
-      </c>
-      <c r="R6" s="48">
+        <v>43967</v>
+      </c>
+      <c r="R6" s="49">
         <f t="shared" si="0"/>
-        <v>43892</v>
-      </c>
-      <c r="S6" s="39">
+        <v>43968</v>
+      </c>
+      <c r="S6" s="48">
         <f t="shared" si="0"/>
-        <v>43893</v>
+        <v>43969</v>
       </c>
       <c r="T6" s="39">
         <f t="shared" si="0"/>
-        <v>43894</v>
+        <v>43970</v>
       </c>
       <c r="U6" s="39">
         <f t="shared" si="0"/>
-        <v>43895</v>
+        <v>43971</v>
       </c>
       <c r="V6" s="39">
         <f t="shared" si="0"/>
-        <v>43896</v>
+        <v>43972</v>
       </c>
       <c r="W6" s="39">
         <f t="shared" si="0"/>
-        <v>43897</v>
-      </c>
-      <c r="X6" s="49">
+        <v>43973</v>
+      </c>
+      <c r="X6" s="39">
         <f t="shared" si="0"/>
-        <v>43898</v>
-      </c>
-      <c r="Y6" s="48">
+        <v>43974</v>
+      </c>
+      <c r="Y6" s="49">
         <f t="shared" si="0"/>
-        <v>43899</v>
-      </c>
-      <c r="Z6" s="39">
+        <v>43975</v>
+      </c>
+      <c r="Z6" s="48">
         <f t="shared" si="0"/>
-        <v>43900</v>
+        <v>43976</v>
       </c>
       <c r="AA6" s="39">
         <f t="shared" si="0"/>
-        <v>43901</v>
+        <v>43977</v>
       </c>
       <c r="AB6" s="39">
         <f t="shared" si="0"/>
-        <v>43902</v>
+        <v>43978</v>
       </c>
       <c r="AC6" s="39">
         <f t="shared" si="0"/>
-        <v>43903</v>
+        <v>43979</v>
       </c>
       <c r="AD6" s="39">
         <f t="shared" si="0"/>
-        <v>43904</v>
-      </c>
-      <c r="AE6" s="49">
+        <v>43980</v>
+      </c>
+      <c r="AE6" s="39">
         <f t="shared" si="0"/>
-        <v>43905</v>
-      </c>
-      <c r="AF6" s="48">
+        <v>43981</v>
+      </c>
+      <c r="AF6" s="49">
         <f t="shared" si="0"/>
-        <v>43906</v>
-      </c>
-      <c r="AG6" s="39">
+        <v>43982</v>
+      </c>
+      <c r="AG6" s="48">
         <f t="shared" si="0"/>
-        <v>43907</v>
+        <v>43983</v>
       </c>
       <c r="AH6" s="39">
         <f t="shared" si="0"/>
-        <v>43908</v>
+        <v>43984</v>
       </c>
       <c r="AI6" s="39">
         <f t="shared" si="0"/>
-        <v>43909</v>
+        <v>43985</v>
       </c>
       <c r="AJ6" s="39">
         <f t="shared" si="0"/>
-        <v>43910</v>
+        <v>43986</v>
       </c>
       <c r="AK6" s="39">
         <f t="shared" si="0"/>
-        <v>43911</v>
-      </c>
-      <c r="AL6" s="49">
+        <v>43987</v>
+      </c>
+      <c r="AL6" s="39">
         <f t="shared" si="0"/>
-        <v>43912</v>
-      </c>
-      <c r="AM6" s="48">
+        <v>43988</v>
+      </c>
+      <c r="AM6" s="49">
         <f t="shared" si="0"/>
-        <v>43913</v>
-      </c>
-      <c r="AN6" s="39">
+        <v>43989</v>
+      </c>
+      <c r="AN6" s="48">
         <f t="shared" si="0"/>
-        <v>43914</v>
+        <v>43990</v>
       </c>
       <c r="AO6" s="39">
         <f t="shared" si="0"/>
-        <v>43915</v>
+        <v>43991</v>
       </c>
       <c r="AP6" s="39">
         <f t="shared" si="0"/>
-        <v>43916</v>
+        <v>43992</v>
       </c>
       <c r="AQ6" s="39">
         <f t="shared" si="0"/>
-        <v>43917</v>
+        <v>43993</v>
       </c>
       <c r="AR6" s="39">
-        <f t="shared" ref="AR6:BN6" si="1">AQ6+1</f>
-        <v>43918</v>
-      </c>
-      <c r="AS6" s="49">
+        <f t="shared" si="0"/>
+        <v>43994</v>
+      </c>
+      <c r="AS6" s="39">
+        <f t="shared" ref="AS6:BO6" si="1">AR6+1</f>
+        <v>43995</v>
+      </c>
+      <c r="AT6" s="49">
         <f t="shared" si="1"/>
-        <v>43919</v>
-      </c>
-      <c r="AT6" s="48">
+        <v>43996</v>
+      </c>
+      <c r="AU6" s="48">
         <f t="shared" si="1"/>
-        <v>43920</v>
-      </c>
-      <c r="AU6" s="39">
-        <f t="shared" si="1"/>
-        <v>43921</v>
+        <v>43997</v>
       </c>
       <c r="AV6" s="39">
         <f t="shared" si="1"/>
-        <v>43922</v>
+        <v>43998</v>
       </c>
       <c r="AW6" s="39">
         <f t="shared" si="1"/>
-        <v>43923</v>
+        <v>43999</v>
       </c>
       <c r="AX6" s="39">
         <f t="shared" si="1"/>
-        <v>43924</v>
+        <v>44000</v>
       </c>
       <c r="AY6" s="39">
         <f t="shared" si="1"/>
-        <v>43925</v>
-      </c>
-      <c r="AZ6" s="49">
+        <v>44001</v>
+      </c>
+      <c r="AZ6" s="39">
         <f t="shared" si="1"/>
-        <v>43926</v>
-      </c>
-      <c r="BA6" s="48">
+        <v>44002</v>
+      </c>
+      <c r="BA6" s="49">
         <f t="shared" si="1"/>
-        <v>43927</v>
-      </c>
-      <c r="BB6" s="39">
+        <v>44003</v>
+      </c>
+      <c r="BB6" s="48">
         <f t="shared" si="1"/>
-        <v>43928</v>
+        <v>44004</v>
       </c>
       <c r="BC6" s="39">
         <f t="shared" si="1"/>
-        <v>43929</v>
+        <v>44005</v>
       </c>
       <c r="BD6" s="39">
         <f t="shared" si="1"/>
-        <v>43930</v>
+        <v>44006</v>
       </c>
       <c r="BE6" s="39">
         <f t="shared" si="1"/>
-        <v>43931</v>
+        <v>44007</v>
       </c>
       <c r="BF6" s="39">
         <f t="shared" si="1"/>
-        <v>43932</v>
-      </c>
-      <c r="BG6" s="49">
+        <v>44008</v>
+      </c>
+      <c r="BG6" s="39">
         <f t="shared" si="1"/>
-        <v>43933</v>
-      </c>
-      <c r="BH6" s="48">
+        <v>44009</v>
+      </c>
+      <c r="BH6" s="49">
         <f t="shared" si="1"/>
-        <v>43934</v>
-      </c>
-      <c r="BI6" s="39">
+        <v>44010</v>
+      </c>
+      <c r="BI6" s="48">
         <f t="shared" si="1"/>
-        <v>43935</v>
+        <v>44011</v>
       </c>
       <c r="BJ6" s="39">
         <f t="shared" si="1"/>
-        <v>43936</v>
+        <v>44012</v>
       </c>
       <c r="BK6" s="39">
         <f t="shared" si="1"/>
-        <v>43937</v>
+        <v>44013</v>
       </c>
       <c r="BL6" s="39">
         <f t="shared" si="1"/>
-        <v>43938</v>
+        <v>44014</v>
       </c>
       <c r="BM6" s="39">
         <f t="shared" si="1"/>
-        <v>43939</v>
-      </c>
-      <c r="BN6" s="49">
+        <v>44015</v>
+      </c>
+      <c r="BN6" s="39">
         <f t="shared" si="1"/>
-        <v>43940</v>
+        <v>44016</v>
+      </c>
+      <c r="BO6" s="49">
+        <f t="shared" si="1"/>
+        <v>44017</v>
+      </c>
+      <c r="BP6" s="48">
+        <f t="shared" ref="BP6" si="2">BO6+1</f>
+        <v>44018</v>
+      </c>
+      <c r="BQ6" s="39">
+        <f t="shared" ref="BQ6" si="3">BP6+1</f>
+        <v>44019</v>
+      </c>
+      <c r="BR6" s="39">
+        <f t="shared" ref="BR6" si="4">BQ6+1</f>
+        <v>44020</v>
+      </c>
+      <c r="BS6" s="39">
+        <f t="shared" ref="BS6" si="5">BR6+1</f>
+        <v>44021</v>
+      </c>
+      <c r="BT6" s="39">
+        <f t="shared" ref="BT6" si="6">BS6+1</f>
+        <v>44022</v>
+      </c>
+      <c r="BU6" s="39">
+        <f t="shared" ref="BU6" si="7">BT6+1</f>
+        <v>44023</v>
+      </c>
+      <c r="BV6" s="49">
+        <f t="shared" ref="BV6" si="8">BU6+1</f>
+        <v>44024</v>
       </c>
     </row>
-    <row r="7" spans="1:66" s="78" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:74" s="78" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="70" t="s">
         <v>0</v>
       </c>
@@ -2758,248 +2844,279 @@
       <c r="D7" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="74" t="s">
+      <c r="E7" s="73" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="74" t="s">
+      <c r="G7" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="72" t="s">
+      <c r="H7" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="72" t="s">
+      <c r="I7" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="72" t="s">
+      <c r="J7" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="72"/>
-      <c r="K7" s="75" t="str">
-        <f t="shared" ref="K7:AP7" si="2">CHOOSE(WEEKDAY(K6,1),"S","M","T","W","T","F","S")</f>
+      <c r="K7" s="72"/>
+      <c r="L7" s="75" t="str">
+        <f t="shared" ref="L7:AQ7" si="9">CHOOSE(WEEKDAY(L6,1),"S","M","T","W","T","F","S")</f>
         <v>M</v>
       </c>
-      <c r="L7" s="76" t="str">
-        <f t="shared" si="2"/>
+      <c r="M7" s="76" t="str">
+        <f t="shared" si="9"/>
         <v>T</v>
       </c>
-      <c r="M7" s="76" t="str">
-        <f t="shared" si="2"/>
+      <c r="N7" s="76" t="str">
+        <f t="shared" si="9"/>
         <v>W</v>
       </c>
-      <c r="N7" s="76" t="str">
-        <f t="shared" si="2"/>
+      <c r="O7" s="76" t="str">
+        <f t="shared" si="9"/>
         <v>T</v>
       </c>
-      <c r="O7" s="76" t="str">
-        <f t="shared" si="2"/>
+      <c r="P7" s="76" t="str">
+        <f t="shared" si="9"/>
         <v>F</v>
       </c>
-      <c r="P7" s="76" t="str">
-        <f t="shared" si="2"/>
+      <c r="Q7" s="76" t="str">
+        <f t="shared" si="9"/>
         <v>S</v>
       </c>
-      <c r="Q7" s="77" t="str">
-        <f t="shared" si="2"/>
+      <c r="R7" s="77" t="str">
+        <f t="shared" si="9"/>
         <v>S</v>
       </c>
-      <c r="R7" s="75" t="str">
-        <f t="shared" si="2"/>
+      <c r="S7" s="75" t="str">
+        <f t="shared" si="9"/>
         <v>M</v>
       </c>
-      <c r="S7" s="76" t="str">
-        <f t="shared" si="2"/>
+      <c r="T7" s="76" t="str">
+        <f t="shared" si="9"/>
         <v>T</v>
       </c>
-      <c r="T7" s="76" t="str">
-        <f t="shared" si="2"/>
+      <c r="U7" s="76" t="str">
+        <f t="shared" si="9"/>
         <v>W</v>
       </c>
-      <c r="U7" s="76" t="str">
-        <f t="shared" si="2"/>
+      <c r="V7" s="76" t="str">
+        <f t="shared" si="9"/>
         <v>T</v>
       </c>
-      <c r="V7" s="76" t="str">
-        <f t="shared" si="2"/>
+      <c r="W7" s="76" t="str">
+        <f t="shared" si="9"/>
         <v>F</v>
       </c>
-      <c r="W7" s="76" t="str">
-        <f t="shared" si="2"/>
+      <c r="X7" s="76" t="str">
+        <f t="shared" si="9"/>
         <v>S</v>
       </c>
-      <c r="X7" s="77" t="str">
-        <f t="shared" si="2"/>
+      <c r="Y7" s="77" t="str">
+        <f t="shared" si="9"/>
         <v>S</v>
       </c>
-      <c r="Y7" s="75" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z7" s="75" t="str">
+        <f t="shared" si="9"/>
         <v>M</v>
       </c>
-      <c r="Z7" s="76" t="str">
-        <f t="shared" si="2"/>
+      <c r="AA7" s="76" t="str">
+        <f t="shared" si="9"/>
         <v>T</v>
       </c>
-      <c r="AA7" s="76" t="str">
-        <f t="shared" si="2"/>
+      <c r="AB7" s="76" t="str">
+        <f t="shared" si="9"/>
         <v>W</v>
       </c>
-      <c r="AB7" s="76" t="str">
-        <f t="shared" si="2"/>
+      <c r="AC7" s="76" t="str">
+        <f t="shared" si="9"/>
         <v>T</v>
       </c>
-      <c r="AC7" s="76" t="str">
-        <f t="shared" si="2"/>
+      <c r="AD7" s="76" t="str">
+        <f t="shared" si="9"/>
         <v>F</v>
       </c>
-      <c r="AD7" s="76" t="str">
-        <f t="shared" si="2"/>
+      <c r="AE7" s="76" t="str">
+        <f t="shared" si="9"/>
         <v>S</v>
       </c>
-      <c r="AE7" s="77" t="str">
-        <f t="shared" si="2"/>
+      <c r="AF7" s="77" t="str">
+        <f t="shared" si="9"/>
         <v>S</v>
       </c>
-      <c r="AF7" s="75" t="str">
-        <f t="shared" si="2"/>
+      <c r="AG7" s="75" t="str">
+        <f t="shared" si="9"/>
         <v>M</v>
       </c>
-      <c r="AG7" s="76" t="str">
-        <f t="shared" si="2"/>
+      <c r="AH7" s="76" t="str">
+        <f t="shared" si="9"/>
         <v>T</v>
       </c>
-      <c r="AH7" s="76" t="str">
-        <f t="shared" si="2"/>
+      <c r="AI7" s="76" t="str">
+        <f t="shared" si="9"/>
         <v>W</v>
       </c>
-      <c r="AI7" s="76" t="str">
-        <f t="shared" si="2"/>
+      <c r="AJ7" s="76" t="str">
+        <f t="shared" si="9"/>
         <v>T</v>
       </c>
-      <c r="AJ7" s="76" t="str">
-        <f t="shared" si="2"/>
+      <c r="AK7" s="76" t="str">
+        <f t="shared" si="9"/>
         <v>F</v>
       </c>
-      <c r="AK7" s="76" t="str">
-        <f t="shared" si="2"/>
+      <c r="AL7" s="76" t="str">
+        <f t="shared" si="9"/>
         <v>S</v>
       </c>
-      <c r="AL7" s="77" t="str">
-        <f t="shared" si="2"/>
+      <c r="AM7" s="77" t="str">
+        <f t="shared" si="9"/>
         <v>S</v>
       </c>
-      <c r="AM7" s="75" t="str">
-        <f t="shared" si="2"/>
+      <c r="AN7" s="75" t="str">
+        <f t="shared" si="9"/>
         <v>M</v>
       </c>
-      <c r="AN7" s="76" t="str">
-        <f t="shared" si="2"/>
+      <c r="AO7" s="76" t="str">
+        <f t="shared" si="9"/>
         <v>T</v>
       </c>
-      <c r="AO7" s="76" t="str">
-        <f t="shared" si="2"/>
+      <c r="AP7" s="76" t="str">
+        <f t="shared" si="9"/>
         <v>W</v>
       </c>
-      <c r="AP7" s="76" t="str">
-        <f t="shared" si="2"/>
+      <c r="AQ7" s="76" t="str">
+        <f t="shared" si="9"/>
         <v>T</v>
       </c>
-      <c r="AQ7" s="76" t="str">
-        <f t="shared" ref="AQ7:BN7" si="3">CHOOSE(WEEKDAY(AQ6,1),"S","M","T","W","T","F","S")</f>
+      <c r="AR7" s="76" t="str">
+        <f t="shared" ref="AR7:BO7" si="10">CHOOSE(WEEKDAY(AR6,1),"S","M","T","W","T","F","S")</f>
         <v>F</v>
       </c>
-      <c r="AR7" s="76" t="str">
-        <f t="shared" si="3"/>
+      <c r="AS7" s="76" t="str">
+        <f t="shared" si="10"/>
         <v>S</v>
       </c>
-      <c r="AS7" s="77" t="str">
-        <f t="shared" si="3"/>
+      <c r="AT7" s="77" t="str">
+        <f t="shared" si="10"/>
         <v>S</v>
       </c>
-      <c r="AT7" s="75" t="str">
-        <f t="shared" si="3"/>
+      <c r="AU7" s="75" t="str">
+        <f t="shared" si="10"/>
         <v>M</v>
       </c>
-      <c r="AU7" s="76" t="str">
-        <f t="shared" si="3"/>
+      <c r="AV7" s="76" t="str">
+        <f t="shared" si="10"/>
         <v>T</v>
       </c>
-      <c r="AV7" s="76" t="str">
-        <f t="shared" si="3"/>
+      <c r="AW7" s="76" t="str">
+        <f t="shared" si="10"/>
         <v>W</v>
       </c>
-      <c r="AW7" s="76" t="str">
-        <f t="shared" si="3"/>
+      <c r="AX7" s="76" t="str">
+        <f t="shared" si="10"/>
         <v>T</v>
       </c>
-      <c r="AX7" s="76" t="str">
-        <f t="shared" si="3"/>
+      <c r="AY7" s="76" t="str">
+        <f t="shared" si="10"/>
         <v>F</v>
       </c>
-      <c r="AY7" s="76" t="str">
-        <f t="shared" si="3"/>
+      <c r="AZ7" s="76" t="str">
+        <f t="shared" si="10"/>
         <v>S</v>
       </c>
-      <c r="AZ7" s="77" t="str">
-        <f t="shared" si="3"/>
+      <c r="BA7" s="77" t="str">
+        <f t="shared" si="10"/>
         <v>S</v>
       </c>
-      <c r="BA7" s="75" t="str">
-        <f t="shared" si="3"/>
+      <c r="BB7" s="75" t="str">
+        <f t="shared" si="10"/>
         <v>M</v>
       </c>
-      <c r="BB7" s="76" t="str">
-        <f t="shared" si="3"/>
+      <c r="BC7" s="76" t="str">
+        <f t="shared" si="10"/>
         <v>T</v>
       </c>
-      <c r="BC7" s="76" t="str">
-        <f t="shared" si="3"/>
+      <c r="BD7" s="76" t="str">
+        <f t="shared" si="10"/>
         <v>W</v>
       </c>
-      <c r="BD7" s="76" t="str">
-        <f t="shared" si="3"/>
+      <c r="BE7" s="76" t="str">
+        <f t="shared" si="10"/>
         <v>T</v>
       </c>
-      <c r="BE7" s="76" t="str">
-        <f t="shared" si="3"/>
+      <c r="BF7" s="76" t="str">
+        <f t="shared" si="10"/>
         <v>F</v>
       </c>
-      <c r="BF7" s="76" t="str">
-        <f t="shared" si="3"/>
+      <c r="BG7" s="76" t="str">
+        <f t="shared" si="10"/>
         <v>S</v>
       </c>
-      <c r="BG7" s="77" t="str">
-        <f t="shared" si="3"/>
+      <c r="BH7" s="77" t="str">
+        <f t="shared" si="10"/>
         <v>S</v>
       </c>
-      <c r="BH7" s="75" t="str">
-        <f t="shared" si="3"/>
+      <c r="BI7" s="75" t="str">
+        <f t="shared" si="10"/>
         <v>M</v>
       </c>
-      <c r="BI7" s="76" t="str">
-        <f t="shared" si="3"/>
+      <c r="BJ7" s="76" t="str">
+        <f t="shared" si="10"/>
         <v>T</v>
       </c>
-      <c r="BJ7" s="76" t="str">
-        <f t="shared" si="3"/>
+      <c r="BK7" s="76" t="str">
+        <f t="shared" si="10"/>
         <v>W</v>
       </c>
-      <c r="BK7" s="76" t="str">
-        <f t="shared" si="3"/>
+      <c r="BL7" s="76" t="str">
+        <f t="shared" si="10"/>
         <v>T</v>
       </c>
-      <c r="BL7" s="76" t="str">
-        <f t="shared" si="3"/>
+      <c r="BM7" s="76" t="str">
+        <f t="shared" si="10"/>
         <v>F</v>
       </c>
-      <c r="BM7" s="76" t="str">
-        <f t="shared" si="3"/>
+      <c r="BN7" s="76" t="str">
+        <f t="shared" si="10"/>
         <v>S</v>
       </c>
-      <c r="BN7" s="77" t="str">
-        <f t="shared" si="3"/>
+      <c r="BO7" s="77" t="str">
+        <f t="shared" si="10"/>
         <v>S</v>
       </c>
+      <c r="BP7" s="75" t="str">
+        <f t="shared" ref="BP7:BV7" si="11">CHOOSE(WEEKDAY(BP6,1),"S","M","T","W","T","F","S")</f>
+        <v>M</v>
+      </c>
+      <c r="BQ7" s="76" t="str">
+        <f t="shared" si="11"/>
+        <v>T</v>
+      </c>
+      <c r="BR7" s="76" t="str">
+        <f t="shared" si="11"/>
+        <v>W</v>
+      </c>
+      <c r="BS7" s="76" t="str">
+        <f t="shared" si="11"/>
+        <v>T</v>
+      </c>
+      <c r="BT7" s="76" t="str">
+        <f t="shared" si="11"/>
+        <v>F</v>
+      </c>
+      <c r="BU7" s="76" t="str">
+        <f t="shared" si="11"/>
+        <v>S</v>
+      </c>
+      <c r="BV7" s="77" t="str">
+        <f t="shared" si="11"/>
+        <v>S</v>
+      </c>
     </row>
-    <row r="8" spans="1:66" s="22" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:74" s="22" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="40" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>1</v>
@@ -3009,18 +3126,18 @@
       </c>
       <c r="C8" s="42"/>
       <c r="D8" s="43"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="69">
+      <c r="E8" s="43"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="69">
         <v>43912</v>
       </c>
-      <c r="G8" s="45"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="47" t="str">
-        <f t="shared" ref="I8:I39" si="4">IF(OR(F8=0,E8=0)," - ",NETWORKDAYS(E8,F8))</f>
+      <c r="H8" s="45"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="47" t="str">
+        <f t="shared" ref="J8:J39" si="12">IF(OR(G8=0,F8=0)," - ",NETWORKDAYS(F8,G8))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J8" s="50"/>
-      <c r="K8" s="60"/>
+      <c r="K8" s="50"/>
       <c r="L8" s="60"/>
       <c r="M8" s="60"/>
       <c r="N8" s="60"/>
@@ -3076,38 +3193,48 @@
       <c r="BL8" s="60"/>
       <c r="BM8" s="60"/>
       <c r="BN8" s="60"/>
+      <c r="BO8" s="60"/>
+      <c r="BP8" s="60"/>
+      <c r="BQ8" s="60"/>
+      <c r="BR8" s="60"/>
+      <c r="BS8" s="60"/>
+      <c r="BT8" s="60"/>
+      <c r="BU8" s="60"/>
+      <c r="BV8" s="60"/>
     </row>
-    <row r="9" spans="1:66" s="28" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:74" s="28" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="27" t="str">
-        <f t="shared" ref="A9:A13" si="5">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A9:A16" si="13">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.1</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C9" s="28" t="s">
         <v>20</v>
       </c>
       <c r="D9" s="81"/>
-      <c r="E9" s="56">
+      <c r="E9" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="56">
         <v>43895</v>
       </c>
-      <c r="F9" s="57">
-        <f>IF(ISBLANK(E9)," - ",IF(G9=0,E9,E9+G9-1))</f>
+      <c r="G9" s="57">
+        <f>IF(ISBLANK(F9)," - ",IF(H9=0,F9,F9+H9-1))</f>
         <v>43901</v>
       </c>
-      <c r="G9" s="29">
+      <c r="H9" s="29">
         <v>7</v>
       </c>
-      <c r="H9" s="30">
+      <c r="I9" s="30">
         <v>1</v>
       </c>
-      <c r="I9" s="31">
-        <f>IF(OR(F9=0,E9=0)," - ",NETWORKDAYS(E9,F9))</f>
+      <c r="J9" s="31">
+        <f>IF(OR(G9=0,F9=0)," - ",NETWORKDAYS(F9,G9))</f>
         <v>5</v>
       </c>
-      <c r="J9" s="51"/>
-      <c r="K9" s="61"/>
+      <c r="K9" s="51"/>
       <c r="L9" s="61"/>
       <c r="M9" s="61"/>
       <c r="N9" s="61"/>
@@ -3163,10 +3290,18 @@
       <c r="BL9" s="61"/>
       <c r="BM9" s="61"/>
       <c r="BN9" s="61"/>
+      <c r="BO9" s="61"/>
+      <c r="BP9" s="61"/>
+      <c r="BQ9" s="61"/>
+      <c r="BR9" s="61"/>
+      <c r="BS9" s="61"/>
+      <c r="BT9" s="61"/>
+      <c r="BU9" s="61"/>
+      <c r="BV9" s="61"/>
     </row>
-    <row r="10" spans="1:66" s="28" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:74" s="28" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="27" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>1.2</v>
       </c>
       <c r="B10" s="80" t="s">
@@ -3176,25 +3311,27 @@
         <v>19</v>
       </c>
       <c r="D10" s="81"/>
-      <c r="E10" s="56">
+      <c r="E10" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="56">
         <v>43886</v>
       </c>
-      <c r="F10" s="57">
-        <f t="shared" ref="F10:F30" si="6">IF(ISBLANK(E10)," - ",IF(G10=0,E10,E10+G10-1))</f>
+      <c r="G10" s="57">
+        <f t="shared" ref="G10:G30" si="14">IF(ISBLANK(F10)," - ",IF(H10=0,F10,F10+H10-1))</f>
         <v>43890</v>
       </c>
-      <c r="G10" s="29">
+      <c r="H10" s="29">
         <v>5</v>
       </c>
-      <c r="H10" s="30">
+      <c r="I10" s="30">
         <v>1</v>
       </c>
-      <c r="I10" s="31">
-        <f t="shared" si="4"/>
+      <c r="J10" s="31">
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
-      <c r="J10" s="51"/>
-      <c r="K10" s="61"/>
+      <c r="K10" s="51"/>
       <c r="L10" s="61"/>
       <c r="M10" s="61"/>
       <c r="N10" s="61"/>
@@ -3250,10 +3387,18 @@
       <c r="BL10" s="61"/>
       <c r="BM10" s="61"/>
       <c r="BN10" s="61"/>
+      <c r="BO10" s="61"/>
+      <c r="BP10" s="61"/>
+      <c r="BQ10" s="61"/>
+      <c r="BR10" s="61"/>
+      <c r="BS10" s="61"/>
+      <c r="BT10" s="61"/>
+      <c r="BU10" s="61"/>
+      <c r="BV10" s="61"/>
     </row>
-    <row r="11" spans="1:66" s="28" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:74" s="28" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="27" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>1.3</v>
       </c>
       <c r="B11" s="80" t="s">
@@ -3263,28 +3408,30 @@
         <v>20</v>
       </c>
       <c r="D11" s="81"/>
-      <c r="E11" s="56">
+      <c r="E11" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="56">
         <v>43891</v>
       </c>
-      <c r="F11" s="57">
-        <f t="shared" si="6"/>
+      <c r="G11" s="57">
+        <f t="shared" si="14"/>
         <v>43894</v>
       </c>
-      <c r="G11" s="29">
+      <c r="H11" s="29">
         <v>4</v>
       </c>
-      <c r="H11" s="30">
+      <c r="I11" s="30">
         <v>1</v>
       </c>
-      <c r="I11" s="31">
-        <f t="shared" si="4"/>
+      <c r="J11" s="31">
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="J11" s="51"/>
-      <c r="K11" s="61"/>
+      <c r="K11" s="51"/>
       <c r="L11" s="61"/>
-      <c r="M11" s="62"/>
-      <c r="N11" s="61"/>
+      <c r="M11" s="61"/>
+      <c r="N11" s="62"/>
       <c r="O11" s="61"/>
       <c r="P11" s="61"/>
       <c r="Q11" s="61"/>
@@ -3337,10 +3484,18 @@
       <c r="BL11" s="61"/>
       <c r="BM11" s="61"/>
       <c r="BN11" s="61"/>
+      <c r="BO11" s="61"/>
+      <c r="BP11" s="61"/>
+      <c r="BQ11" s="61"/>
+      <c r="BR11" s="61"/>
+      <c r="BS11" s="61"/>
+      <c r="BT11" s="61"/>
+      <c r="BU11" s="61"/>
+      <c r="BV11" s="61"/>
     </row>
-    <row r="12" spans="1:66" s="28" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:74" s="28" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A12" s="27" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>1.4</v>
       </c>
       <c r="B12" s="80" t="s">
@@ -3350,25 +3505,27 @@
         <v>24</v>
       </c>
       <c r="D12" s="81"/>
-      <c r="E12" s="56">
+      <c r="E12" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="56">
         <v>43885</v>
       </c>
-      <c r="F12" s="57">
-        <f>IF(ISBLANK(E12)," - ",IF(G12=0,E12,E12+G12-1))</f>
+      <c r="G12" s="57">
+        <f>IF(ISBLANK(F12)," - ",IF(H12=0,F12,F12+H12-1))</f>
         <v>43886</v>
       </c>
-      <c r="G12" s="29">
+      <c r="H12" s="29">
         <v>2</v>
       </c>
-      <c r="H12" s="30">
+      <c r="I12" s="30">
         <v>1</v>
       </c>
-      <c r="I12" s="31">
-        <f>IF(OR(F12=0,E12=0)," - ",NETWORKDAYS(E12,F12))</f>
+      <c r="J12" s="31">
+        <f>IF(OR(G12=0,F12=0)," - ",NETWORKDAYS(F12,G12))</f>
         <v>2</v>
       </c>
-      <c r="J12" s="51"/>
-      <c r="K12" s="61"/>
+      <c r="K12" s="51"/>
       <c r="L12" s="61"/>
       <c r="M12" s="61"/>
       <c r="N12" s="61"/>
@@ -3424,10 +3581,18 @@
       <c r="BL12" s="61"/>
       <c r="BM12" s="61"/>
       <c r="BN12" s="61"/>
+      <c r="BO12" s="61"/>
+      <c r="BP12" s="61"/>
+      <c r="BQ12" s="61"/>
+      <c r="BR12" s="61"/>
+      <c r="BS12" s="61"/>
+      <c r="BT12" s="61"/>
+      <c r="BU12" s="61"/>
+      <c r="BV12" s="61"/>
     </row>
-    <row r="13" spans="1:66" s="28" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:74" s="28" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="27" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>1.5</v>
       </c>
       <c r="B13" s="80" t="s">
@@ -3437,25 +3602,27 @@
         <v>23</v>
       </c>
       <c r="D13" s="81"/>
-      <c r="E13" s="56">
+      <c r="E13" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="56">
         <v>43895</v>
       </c>
-      <c r="F13" s="57">
-        <f>IF(ISBLANK(E13)," - ",IF(G13=0,E13,E13+G13-1))</f>
+      <c r="G13" s="57">
+        <f>IF(ISBLANK(F13)," - ",IF(H13=0,F13,F13+H13-1))</f>
         <v>43900</v>
       </c>
-      <c r="G13" s="29">
+      <c r="H13" s="29">
         <v>6</v>
       </c>
-      <c r="H13" s="30">
+      <c r="I13" s="30">
         <v>1</v>
       </c>
-      <c r="I13" s="31">
-        <f>IF(OR(F13=0,E13=0)," - ",NETWORKDAYS(E13,F13))</f>
+      <c r="J13" s="31">
+        <f>IF(OR(G13=0,F13=0)," - ",NETWORKDAYS(F13,G13))</f>
         <v>4</v>
       </c>
-      <c r="J13" s="51"/>
-      <c r="K13" s="61"/>
+      <c r="K13" s="51"/>
       <c r="L13" s="61"/>
       <c r="M13" s="61"/>
       <c r="N13" s="61"/>
@@ -3511,37 +3678,48 @@
       <c r="BL13" s="61"/>
       <c r="BM13" s="61"/>
       <c r="BN13" s="61"/>
+      <c r="BO13" s="61"/>
+      <c r="BP13" s="61"/>
+      <c r="BQ13" s="61"/>
+      <c r="BR13" s="61"/>
+      <c r="BS13" s="61"/>
+      <c r="BT13" s="61"/>
+      <c r="BU13" s="61"/>
+      <c r="BV13" s="61"/>
     </row>
-    <row r="14" spans="1:66" s="28" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A14" s="27">
+    <row r="14" spans="1:74" s="28" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="27" t="str">
+        <f t="shared" si="13"/>
         <v>1.6</v>
       </c>
       <c r="B14" s="80" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D14" s="86"/>
-      <c r="E14" s="56">
+      <c r="E14" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="56">
+        <v>43901</v>
+      </c>
+      <c r="G14" s="57">
+        <f>IF(ISBLANK(F14)," - ",IF(H14=0,F14,F14+H14-1))</f>
         <v>43905</v>
       </c>
-      <c r="F14" s="57">
-        <f>IF(ISBLANK(E14)," - ",IF(G14=0,E14,E14+G14-1))</f>
-        <v>43962</v>
-      </c>
-      <c r="G14" s="29">
-        <v>58</v>
-      </c>
-      <c r="H14" s="30">
+      <c r="H14" s="29">
+        <v>5</v>
+      </c>
+      <c r="I14" s="91">
         <v>1</v>
       </c>
-      <c r="I14" s="31">
-        <f>IF(OR(F14=0,E14=0)," - ",NETWORKDAYS(E14,F14))</f>
-        <v>41</v>
-      </c>
-      <c r="J14" s="51"/>
-      <c r="K14" s="61"/>
+      <c r="J14" s="31">
+        <f>IF(OR(G14=0,F14=0)," - ",NETWORKDAYS(F14,G14))</f>
+        <v>3</v>
+      </c>
+      <c r="K14" s="51"/>
       <c r="L14" s="61"/>
       <c r="M14" s="61"/>
       <c r="N14" s="61"/>
@@ -3597,35 +3775,48 @@
       <c r="BL14" s="61"/>
       <c r="BM14" s="61"/>
       <c r="BN14" s="61"/>
+      <c r="BO14" s="61"/>
+      <c r="BP14" s="61"/>
+      <c r="BQ14" s="61"/>
+      <c r="BR14" s="61"/>
+      <c r="BS14" s="61"/>
+      <c r="BT14" s="61"/>
+      <c r="BU14" s="61"/>
+      <c r="BV14" s="61"/>
     </row>
-    <row r="15" spans="1:66" s="28" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A15" s="27">
+    <row r="15" spans="1:74" s="28" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="27" t="str">
+        <f t="shared" si="13"/>
         <v>1.7</v>
       </c>
       <c r="B15" s="80" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="D15" s="86"/>
-      <c r="E15" s="56">
-        <v>43929</v>
-      </c>
-      <c r="F15" s="97">
-        <v>43929</v>
-      </c>
-      <c r="G15" s="99">
+      <c r="E15" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="56">
+        <v>43905</v>
+      </c>
+      <c r="G15" s="57">
+        <f>IF(ISBLANK(F15)," - ",IF(H15=0,F15,F15+H15-1))</f>
+        <v>43962</v>
+      </c>
+      <c r="H15" s="29">
+        <v>58</v>
+      </c>
+      <c r="I15" s="30">
         <v>1</v>
       </c>
-      <c r="H15" s="100">
-        <v>1</v>
-      </c>
-      <c r="I15" s="101">
-        <v>1</v>
-      </c>
-      <c r="J15" s="102"/>
-      <c r="K15" s="61"/>
+      <c r="J15" s="31">
+        <f>IF(OR(G15=0,F15=0)," - ",NETWORKDAYS(F15,G15))</f>
+        <v>41</v>
+      </c>
+      <c r="K15" s="51"/>
       <c r="L15" s="61"/>
       <c r="M15" s="61"/>
       <c r="N15" s="61"/>
@@ -3681,202 +3872,228 @@
       <c r="BL15" s="61"/>
       <c r="BM15" s="61"/>
       <c r="BN15" s="61"/>
+      <c r="BO15" s="61"/>
+      <c r="BP15" s="61"/>
+      <c r="BQ15" s="61"/>
+      <c r="BR15" s="61"/>
+      <c r="BS15" s="61"/>
+      <c r="BT15" s="61"/>
+      <c r="BU15" s="61"/>
+      <c r="BV15" s="61"/>
     </row>
-    <row r="16" spans="1:66" s="22" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="str">
+    <row r="16" spans="1:74" s="28" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+      <c r="A16" s="27" t="str">
+        <f t="shared" si="13"/>
+        <v>1.8</v>
+      </c>
+      <c r="B16" s="80" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="86"/>
+      <c r="E16" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="56">
+        <v>43929</v>
+      </c>
+      <c r="G16" s="88">
+        <v>43929</v>
+      </c>
+      <c r="H16" s="90">
+        <v>1</v>
+      </c>
+      <c r="I16" s="91">
+        <v>1</v>
+      </c>
+      <c r="J16" s="92">
+        <v>1</v>
+      </c>
+      <c r="K16" s="93"/>
+      <c r="L16" s="61"/>
+      <c r="M16" s="61"/>
+      <c r="N16" s="61"/>
+      <c r="O16" s="61"/>
+      <c r="P16" s="61"/>
+      <c r="Q16" s="61"/>
+      <c r="R16" s="61"/>
+      <c r="S16" s="61"/>
+      <c r="T16" s="61"/>
+      <c r="U16" s="61"/>
+      <c r="V16" s="61"/>
+      <c r="W16" s="61"/>
+      <c r="X16" s="61"/>
+      <c r="Y16" s="61"/>
+      <c r="Z16" s="61"/>
+      <c r="AA16" s="61"/>
+      <c r="AB16" s="61"/>
+      <c r="AC16" s="61"/>
+      <c r="AD16" s="61"/>
+      <c r="AE16" s="61"/>
+      <c r="AF16" s="61"/>
+      <c r="AG16" s="61"/>
+      <c r="AH16" s="61"/>
+      <c r="AI16" s="61"/>
+      <c r="AJ16" s="61"/>
+      <c r="AK16" s="61"/>
+      <c r="AL16" s="61"/>
+      <c r="AM16" s="61"/>
+      <c r="AN16" s="61"/>
+      <c r="AO16" s="61"/>
+      <c r="AP16" s="61"/>
+      <c r="AQ16" s="61"/>
+      <c r="AR16" s="61"/>
+      <c r="AS16" s="61"/>
+      <c r="AT16" s="61"/>
+      <c r="AU16" s="61"/>
+      <c r="AV16" s="61"/>
+      <c r="AW16" s="61"/>
+      <c r="AX16" s="61"/>
+      <c r="AY16" s="61"/>
+      <c r="AZ16" s="61"/>
+      <c r="BA16" s="61"/>
+      <c r="BB16" s="61"/>
+      <c r="BC16" s="61"/>
+      <c r="BD16" s="61"/>
+      <c r="BE16" s="61"/>
+      <c r="BF16" s="61"/>
+      <c r="BG16" s="61"/>
+      <c r="BH16" s="61"/>
+      <c r="BI16" s="61"/>
+      <c r="BJ16" s="61"/>
+      <c r="BK16" s="61"/>
+      <c r="BL16" s="61"/>
+      <c r="BM16" s="61"/>
+      <c r="BN16" s="61"/>
+      <c r="BO16" s="61"/>
+      <c r="BP16" s="61"/>
+      <c r="BQ16" s="61"/>
+      <c r="BR16" s="61"/>
+      <c r="BS16" s="61"/>
+      <c r="BT16" s="61"/>
+      <c r="BU16" s="61"/>
+      <c r="BV16" s="61"/>
+    </row>
+    <row r="17" spans="1:74" s="22" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A17" s="20" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>2</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B17" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="23"/>
-      <c r="E16" s="58"/>
-      <c r="F16" s="58">
-        <v>43922</v>
-      </c>
-      <c r="G16" s="24"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="26" t="str">
-        <f t="shared" si="4"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="58">
+        <v>43963</v>
+      </c>
+      <c r="H17" s="24"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="26" t="str">
+        <f t="shared" si="12"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J16" s="52"/>
-      <c r="K16" s="63"/>
-      <c r="L16" s="63"/>
-      <c r="M16" s="63"/>
-      <c r="N16" s="63"/>
-      <c r="O16" s="63"/>
-      <c r="P16" s="63"/>
-      <c r="Q16" s="63"/>
-      <c r="R16" s="63"/>
-      <c r="S16" s="63"/>
-      <c r="T16" s="63"/>
-      <c r="U16" s="63"/>
-      <c r="V16" s="63"/>
-      <c r="W16" s="63"/>
-      <c r="X16" s="63"/>
-      <c r="Y16" s="63"/>
-      <c r="Z16" s="63"/>
-      <c r="AA16" s="63"/>
-      <c r="AB16" s="63"/>
-      <c r="AC16" s="63"/>
-      <c r="AD16" s="63"/>
-      <c r="AE16" s="63"/>
-      <c r="AF16" s="63"/>
-      <c r="AG16" s="63"/>
-      <c r="AH16" s="63"/>
-      <c r="AI16" s="63"/>
-      <c r="AJ16" s="63"/>
-      <c r="AK16" s="63"/>
-      <c r="AL16" s="63"/>
-      <c r="AM16" s="63"/>
-      <c r="AN16" s="63"/>
-      <c r="AO16" s="63"/>
-      <c r="AP16" s="63"/>
-      <c r="AQ16" s="63"/>
-      <c r="AR16" s="63"/>
-      <c r="AS16" s="63"/>
-      <c r="AT16" s="63"/>
-      <c r="AU16" s="63"/>
-      <c r="AV16" s="63"/>
-      <c r="AW16" s="63"/>
-      <c r="AX16" s="63"/>
-      <c r="AY16" s="63"/>
-      <c r="AZ16" s="63"/>
-      <c r="BA16" s="63"/>
-      <c r="BB16" s="63"/>
-      <c r="BC16" s="63"/>
-      <c r="BD16" s="63"/>
-      <c r="BE16" s="63"/>
-      <c r="BF16" s="63"/>
-      <c r="BG16" s="63"/>
-      <c r="BH16" s="63"/>
-      <c r="BI16" s="63"/>
-      <c r="BJ16" s="63"/>
-      <c r="BK16" s="63"/>
-      <c r="BL16" s="63"/>
-      <c r="BM16" s="63"/>
-      <c r="BN16" s="63"/>
+      <c r="K17" s="52"/>
+      <c r="L17" s="63"/>
+      <c r="M17" s="63"/>
+      <c r="N17" s="63"/>
+      <c r="O17" s="63"/>
+      <c r="P17" s="63"/>
+      <c r="Q17" s="63"/>
+      <c r="R17" s="63"/>
+      <c r="S17" s="63"/>
+      <c r="T17" s="63"/>
+      <c r="U17" s="63"/>
+      <c r="V17" s="63"/>
+      <c r="W17" s="63"/>
+      <c r="X17" s="63"/>
+      <c r="Y17" s="63"/>
+      <c r="Z17" s="63"/>
+      <c r="AA17" s="63"/>
+      <c r="AB17" s="63"/>
+      <c r="AC17" s="63"/>
+      <c r="AD17" s="63"/>
+      <c r="AE17" s="63"/>
+      <c r="AF17" s="63"/>
+      <c r="AG17" s="63"/>
+      <c r="AH17" s="63"/>
+      <c r="AI17" s="63"/>
+      <c r="AJ17" s="63"/>
+      <c r="AK17" s="63"/>
+      <c r="AL17" s="63"/>
+      <c r="AM17" s="63"/>
+      <c r="AN17" s="63"/>
+      <c r="AO17" s="63"/>
+      <c r="AP17" s="63"/>
+      <c r="AQ17" s="63"/>
+      <c r="AR17" s="63"/>
+      <c r="AS17" s="63"/>
+      <c r="AT17" s="63"/>
+      <c r="AU17" s="63"/>
+      <c r="AV17" s="63"/>
+      <c r="AW17" s="63"/>
+      <c r="AX17" s="63"/>
+      <c r="AY17" s="63"/>
+      <c r="AZ17" s="63"/>
+      <c r="BA17" s="63"/>
+      <c r="BB17" s="63"/>
+      <c r="BC17" s="63"/>
+      <c r="BD17" s="63"/>
+      <c r="BE17" s="63"/>
+      <c r="BF17" s="63"/>
+      <c r="BG17" s="63"/>
+      <c r="BH17" s="63"/>
+      <c r="BI17" s="63"/>
+      <c r="BJ17" s="63"/>
+      <c r="BK17" s="63"/>
+      <c r="BL17" s="63"/>
+      <c r="BM17" s="63"/>
+      <c r="BN17" s="63"/>
+      <c r="BO17" s="63"/>
+      <c r="BP17" s="63"/>
+      <c r="BQ17" s="63"/>
+      <c r="BR17" s="63"/>
+      <c r="BS17" s="63"/>
+      <c r="BT17" s="63"/>
+      <c r="BU17" s="63"/>
+      <c r="BV17" s="63"/>
     </row>
-    <row r="17" spans="1:66" s="28" customFormat="1" ht="36" x14ac:dyDescent="0.2">
-      <c r="A17" s="27" t="str">
-        <f t="shared" ref="A17:A23" si="7">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+    <row r="18" spans="1:74" s="28" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="27" t="str">
+        <f t="shared" ref="A18:A23" si="15">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.1</v>
       </c>
-      <c r="B17" s="80" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="28" t="s">
+      <c r="B18" s="80" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="81"/>
-      <c r="E17" s="56">
-        <v>43919</v>
-      </c>
-      <c r="F17" s="57">
-        <f t="shared" si="6"/>
-        <v>43924</v>
-      </c>
-      <c r="G17" s="29">
+      <c r="D18" s="81"/>
+      <c r="E18" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="56">
+        <v>43933</v>
+      </c>
+      <c r="G18" s="57">
+        <f t="shared" si="14"/>
+        <v>43938</v>
+      </c>
+      <c r="H18" s="29">
         <v>6</v>
       </c>
-      <c r="H17" s="30">
-        <v>0</v>
-      </c>
-      <c r="I17" s="31">
-        <f t="shared" si="4"/>
+      <c r="I18" s="91">
+        <v>1</v>
+      </c>
+      <c r="J18" s="31">
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
-      <c r="J17" s="51"/>
-      <c r="K17" s="61"/>
-      <c r="L17" s="61"/>
-      <c r="M17" s="61"/>
-      <c r="N17" s="61"/>
-      <c r="O17" s="61"/>
-      <c r="P17" s="61"/>
-      <c r="Q17" s="61"/>
-      <c r="R17" s="61"/>
-      <c r="S17" s="61"/>
-      <c r="T17" s="61"/>
-      <c r="U17" s="61"/>
-      <c r="V17" s="61"/>
-      <c r="W17" s="61"/>
-      <c r="X17" s="61"/>
-      <c r="Y17" s="61"/>
-      <c r="Z17" s="61"/>
-      <c r="AA17" s="61"/>
-      <c r="AB17" s="61"/>
-      <c r="AC17" s="61"/>
-      <c r="AD17" s="61"/>
-      <c r="AE17" s="61"/>
-      <c r="AF17" s="61"/>
-      <c r="AG17" s="61"/>
-      <c r="AH17" s="61"/>
-      <c r="AI17" s="61"/>
-      <c r="AJ17" s="61"/>
-      <c r="AK17" s="61"/>
-      <c r="AL17" s="61"/>
-      <c r="AM17" s="61"/>
-      <c r="AN17" s="61"/>
-      <c r="AO17" s="61"/>
-      <c r="AP17" s="61"/>
-      <c r="AQ17" s="61"/>
-      <c r="AR17" s="61"/>
-      <c r="AS17" s="61"/>
-      <c r="AT17" s="61"/>
-      <c r="AU17" s="61"/>
-      <c r="AV17" s="61"/>
-      <c r="AW17" s="61"/>
-      <c r="AX17" s="61"/>
-      <c r="AY17" s="61"/>
-      <c r="AZ17" s="61"/>
-      <c r="BA17" s="61"/>
-      <c r="BB17" s="61"/>
-      <c r="BC17" s="61"/>
-      <c r="BD17" s="61"/>
-      <c r="BE17" s="61"/>
-      <c r="BF17" s="61"/>
-      <c r="BG17" s="61"/>
-      <c r="BH17" s="61"/>
-      <c r="BI17" s="61"/>
-      <c r="BJ17" s="61"/>
-      <c r="BK17" s="61"/>
-      <c r="BL17" s="61"/>
-      <c r="BM17" s="61"/>
-      <c r="BN17" s="61"/>
-    </row>
-    <row r="18" spans="1:66" s="28" customFormat="1" ht="24" x14ac:dyDescent="0.2">
-      <c r="A18" s="27" t="str">
-        <f t="shared" si="7"/>
-        <v>2.2</v>
-      </c>
-      <c r="B18" s="80" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="81"/>
-      <c r="E18" s="56">
-        <v>43919</v>
-      </c>
-      <c r="F18" s="57">
-        <f t="shared" si="6"/>
-        <v>43920</v>
-      </c>
-      <c r="G18" s="29">
-        <v>2</v>
-      </c>
-      <c r="H18" s="30">
-        <v>0</v>
-      </c>
-      <c r="I18" s="31">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J18" s="51"/>
-      <c r="K18" s="61"/>
+      <c r="K18" s="51"/>
       <c r="L18" s="61"/>
       <c r="M18" s="61"/>
       <c r="N18" s="61"/>
@@ -3932,38 +4149,48 @@
       <c r="BL18" s="61"/>
       <c r="BM18" s="61"/>
       <c r="BN18" s="61"/>
+      <c r="BO18" s="61"/>
+      <c r="BP18" s="61"/>
+      <c r="BQ18" s="61"/>
+      <c r="BR18" s="61"/>
+      <c r="BS18" s="61"/>
+      <c r="BT18" s="61"/>
+      <c r="BU18" s="61"/>
+      <c r="BV18" s="61"/>
     </row>
-    <row r="19" spans="1:66" s="28" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:74" s="28" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A19" s="27" t="str">
-        <f t="shared" si="7"/>
-        <v>2.3</v>
+        <f t="shared" si="15"/>
+        <v>2.2</v>
       </c>
       <c r="B19" s="80" t="s">
         <v>25</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D19" s="81"/>
-      <c r="E19" s="56">
-        <v>43919</v>
-      </c>
-      <c r="F19" s="57">
-        <f t="shared" si="6"/>
-        <v>43923</v>
-      </c>
-      <c r="G19" s="29">
-        <v>5</v>
-      </c>
-      <c r="H19" s="30">
-        <v>0</v>
-      </c>
-      <c r="I19" s="31">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="J19" s="51"/>
-      <c r="K19" s="61"/>
+      <c r="E19" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="56">
+        <v>43937</v>
+      </c>
+      <c r="G19" s="57">
+        <f t="shared" si="14"/>
+        <v>43939</v>
+      </c>
+      <c r="H19" s="29">
+        <v>3</v>
+      </c>
+      <c r="I19" s="91">
+        <v>1</v>
+      </c>
+      <c r="J19" s="31">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="K19" s="51"/>
       <c r="L19" s="61"/>
       <c r="M19" s="61"/>
       <c r="N19" s="61"/>
@@ -4019,38 +4246,48 @@
       <c r="BL19" s="61"/>
       <c r="BM19" s="61"/>
       <c r="BN19" s="61"/>
+      <c r="BO19" s="61"/>
+      <c r="BP19" s="61"/>
+      <c r="BQ19" s="61"/>
+      <c r="BR19" s="61"/>
+      <c r="BS19" s="61"/>
+      <c r="BT19" s="61"/>
+      <c r="BU19" s="61"/>
+      <c r="BV19" s="61"/>
     </row>
-    <row r="20" spans="1:66" s="28" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:74" s="28" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A20" s="27" t="str">
-        <f t="shared" si="7"/>
-        <v>2.4</v>
+        <f t="shared" si="15"/>
+        <v>2.3</v>
       </c>
       <c r="B20" s="80" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" s="28" t="s">
         <v>20</v>
       </c>
       <c r="D20" s="81"/>
-      <c r="E20" s="56">
-        <v>43919</v>
-      </c>
-      <c r="F20" s="57">
-        <f t="shared" si="6"/>
-        <v>43924</v>
-      </c>
-      <c r="G20" s="29">
+      <c r="E20" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="56">
+        <v>43940</v>
+      </c>
+      <c r="G20" s="57">
+        <f t="shared" si="14"/>
+        <v>43945</v>
+      </c>
+      <c r="H20" s="29">
         <v>6</v>
       </c>
-      <c r="H20" s="30">
-        <v>0</v>
-      </c>
-      <c r="I20" s="31">
-        <f t="shared" si="4"/>
+      <c r="I20" s="91">
+        <v>1</v>
+      </c>
+      <c r="J20" s="31">
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
-      <c r="J20" s="51"/>
-      <c r="K20" s="61"/>
+      <c r="K20" s="51"/>
       <c r="L20" s="61"/>
       <c r="M20" s="61"/>
       <c r="N20" s="61"/>
@@ -4106,38 +4343,48 @@
       <c r="BL20" s="61"/>
       <c r="BM20" s="61"/>
       <c r="BN20" s="61"/>
+      <c r="BO20" s="61"/>
+      <c r="BP20" s="61"/>
+      <c r="BQ20" s="61"/>
+      <c r="BR20" s="61"/>
+      <c r="BS20" s="61"/>
+      <c r="BT20" s="61"/>
+      <c r="BU20" s="61"/>
+      <c r="BV20" s="61"/>
     </row>
-    <row r="21" spans="1:66" s="28" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:74" s="28" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A21" s="27" t="str">
-        <f t="shared" si="7"/>
-        <v>2.5</v>
+        <f t="shared" si="15"/>
+        <v>2.4</v>
       </c>
       <c r="B21" s="80" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C21" s="28" t="s">
         <v>23</v>
       </c>
       <c r="D21" s="81"/>
-      <c r="E21" s="56">
-        <v>43919</v>
-      </c>
-      <c r="F21" s="57">
-        <f t="shared" si="6"/>
-        <v>43923</v>
-      </c>
-      <c r="G21" s="29">
-        <v>5</v>
-      </c>
-      <c r="H21" s="30">
-        <v>0</v>
-      </c>
-      <c r="I21" s="31">
-        <f t="shared" ref="I21:I22" si="8">IF(OR(F21=0,E21=0)," - ",NETWORKDAYS(E21,F21))</f>
+      <c r="E21" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="56">
+        <v>43950</v>
+      </c>
+      <c r="G21" s="57">
+        <f t="shared" si="14"/>
+        <v>43953</v>
+      </c>
+      <c r="H21" s="29">
         <v>4</v>
       </c>
-      <c r="J21" s="51"/>
-      <c r="K21" s="61"/>
+      <c r="I21" s="91">
+        <v>1</v>
+      </c>
+      <c r="J21" s="31">
+        <f t="shared" ref="J21:J22" si="16">IF(OR(G21=0,F21=0)," - ",NETWORKDAYS(F21,G21))</f>
+        <v>3</v>
+      </c>
+      <c r="K21" s="51"/>
       <c r="L21" s="61"/>
       <c r="M21" s="61"/>
       <c r="N21" s="61"/>
@@ -4193,38 +4440,48 @@
       <c r="BL21" s="61"/>
       <c r="BM21" s="61"/>
       <c r="BN21" s="61"/>
+      <c r="BO21" s="61"/>
+      <c r="BP21" s="61"/>
+      <c r="BQ21" s="61"/>
+      <c r="BR21" s="61"/>
+      <c r="BS21" s="61"/>
+      <c r="BT21" s="61"/>
+      <c r="BU21" s="61"/>
+      <c r="BV21" s="61"/>
     </row>
-    <row r="22" spans="1:66" s="28" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:74" s="28" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="27" t="str">
-        <f t="shared" si="7"/>
-        <v>2.6</v>
+        <f t="shared" si="15"/>
+        <v>2.5</v>
       </c>
       <c r="B22" s="80" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="C22" s="28" t="s">
         <v>22</v>
       </c>
       <c r="D22" s="81"/>
-      <c r="E22" s="56">
-        <v>43919</v>
-      </c>
-      <c r="F22" s="57">
-        <f t="shared" si="6"/>
-        <v>43927</v>
-      </c>
-      <c r="G22" s="29">
-        <v>9</v>
-      </c>
-      <c r="H22" s="30">
-        <v>0</v>
-      </c>
-      <c r="I22" s="31">
-        <f t="shared" si="8"/>
-        <v>6</v>
-      </c>
-      <c r="J22" s="51"/>
-      <c r="K22" s="61"/>
+      <c r="E22" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" s="56">
+        <v>43957</v>
+      </c>
+      <c r="G22" s="57">
+        <f t="shared" si="14"/>
+        <v>43961</v>
+      </c>
+      <c r="H22" s="29">
+        <v>5</v>
+      </c>
+      <c r="I22" s="91">
+        <v>1</v>
+      </c>
+      <c r="J22" s="31">
+        <f t="shared" si="16"/>
+        <v>3</v>
+      </c>
+      <c r="K22" s="51"/>
       <c r="L22" s="61"/>
       <c r="M22" s="61"/>
       <c r="N22" s="61"/>
@@ -4280,38 +4537,48 @@
       <c r="BL22" s="61"/>
       <c r="BM22" s="61"/>
       <c r="BN22" s="61"/>
+      <c r="BO22" s="61"/>
+      <c r="BP22" s="61"/>
+      <c r="BQ22" s="61"/>
+      <c r="BR22" s="61"/>
+      <c r="BS22" s="61"/>
+      <c r="BT22" s="61"/>
+      <c r="BU22" s="61"/>
+      <c r="BV22" s="61"/>
     </row>
-    <row r="23" spans="1:66" s="28" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:74" s="28" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="27" t="str">
-        <f t="shared" si="7"/>
-        <v>2.7</v>
+        <f t="shared" si="15"/>
+        <v>2.6</v>
       </c>
       <c r="B23" s="80" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C23" s="28" t="s">
         <v>24</v>
       </c>
       <c r="D23" s="81"/>
-      <c r="E23" s="56">
-        <v>43919</v>
-      </c>
-      <c r="F23" s="57">
-        <f t="shared" si="6"/>
-        <v>43925</v>
-      </c>
-      <c r="G23" s="29">
-        <v>7</v>
-      </c>
-      <c r="H23" s="30">
-        <v>0</v>
-      </c>
-      <c r="I23" s="31">
-        <f t="shared" si="4"/>
+      <c r="E23" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F23" s="56">
+        <v>43961</v>
+      </c>
+      <c r="G23" s="57">
+        <f t="shared" si="14"/>
+        <v>43965</v>
+      </c>
+      <c r="H23" s="29">
         <v>5</v>
       </c>
-      <c r="J23" s="51"/>
-      <c r="K23" s="61"/>
+      <c r="I23" s="91">
+        <v>1</v>
+      </c>
+      <c r="J23" s="31">
+        <f t="shared" si="12"/>
+        <v>4</v>
+      </c>
+      <c r="K23" s="51"/>
       <c r="L23" s="61"/>
       <c r="M23" s="61"/>
       <c r="N23" s="61"/>
@@ -4367,27 +4634,47 @@
       <c r="BL23" s="61"/>
       <c r="BM23" s="61"/>
       <c r="BN23" s="61"/>
+      <c r="BO23" s="61"/>
+      <c r="BP23" s="61"/>
+      <c r="BQ23" s="61"/>
+      <c r="BR23" s="61"/>
+      <c r="BS23" s="61"/>
+      <c r="BT23" s="61"/>
+      <c r="BU23" s="61"/>
+      <c r="BV23" s="61"/>
     </row>
-    <row r="24" spans="1:66" s="28" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:74" s="28" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="27">
         <v>2.8</v>
       </c>
       <c r="B24" s="80" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D24" s="86"/>
-      <c r="E24" s="97"/>
-      <c r="F24" s="98"/>
-      <c r="G24" s="99"/>
-      <c r="H24" s="100">
-        <v>0</v>
-      </c>
-      <c r="I24" s="101"/>
-      <c r="J24" s="102"/>
-      <c r="K24" s="61"/>
+      <c r="E24" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" s="56">
+        <v>43965</v>
+      </c>
+      <c r="G24" s="89">
+        <f t="shared" si="14"/>
+        <v>43965</v>
+      </c>
+      <c r="H24" s="90">
+        <v>1</v>
+      </c>
+      <c r="I24" s="91">
+        <v>1</v>
+      </c>
+      <c r="J24" s="92">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="K24" s="93"/>
       <c r="L24" s="61"/>
       <c r="M24" s="61"/>
       <c r="N24" s="61"/>
@@ -4443,28 +4730,36 @@
       <c r="BL24" s="61"/>
       <c r="BM24" s="61"/>
       <c r="BN24" s="61"/>
+      <c r="BO24" s="61"/>
+      <c r="BP24" s="61"/>
+      <c r="BQ24" s="61"/>
+      <c r="BR24" s="61"/>
+      <c r="BS24" s="61"/>
+      <c r="BT24" s="61"/>
+      <c r="BU24" s="61"/>
+      <c r="BV24" s="61"/>
     </row>
-    <row r="25" spans="1:66" s="22" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:74" s="22" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>3</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D25" s="23"/>
-      <c r="E25" s="58"/>
-      <c r="F25" s="58">
-        <v>43943</v>
-      </c>
-      <c r="G25" s="24"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="26" t="str">
-        <f t="shared" si="4"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="58">
+        <v>43970</v>
+      </c>
+      <c r="H25" s="24"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="26" t="str">
+        <f t="shared" si="12"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J25" s="52"/>
-      <c r="K25" s="63"/>
+      <c r="K25" s="52"/>
       <c r="L25" s="63"/>
       <c r="M25" s="63"/>
       <c r="N25" s="63"/>
@@ -4520,38 +4815,48 @@
       <c r="BL25" s="63"/>
       <c r="BM25" s="63"/>
       <c r="BN25" s="63"/>
+      <c r="BO25" s="63"/>
+      <c r="BP25" s="63"/>
+      <c r="BQ25" s="63"/>
+      <c r="BR25" s="63"/>
+      <c r="BS25" s="63"/>
+      <c r="BT25" s="63"/>
+      <c r="BU25" s="63"/>
+      <c r="BV25" s="63"/>
     </row>
-    <row r="26" spans="1:66" s="28" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:74" s="28" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A26" s="27" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.1</v>
       </c>
       <c r="B26" s="80" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="28" t="s">
         <v>23</v>
       </c>
       <c r="D26" s="81"/>
-      <c r="E26" s="56">
-        <v>43927</v>
-      </c>
-      <c r="F26" s="57">
-        <f t="shared" si="6"/>
-        <v>43930</v>
-      </c>
-      <c r="G26" s="29">
-        <v>4</v>
-      </c>
-      <c r="H26" s="30">
+      <c r="E26" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="56">
+        <v>43965</v>
+      </c>
+      <c r="G26" s="57">
+        <f t="shared" si="14"/>
+        <v>43967</v>
+      </c>
+      <c r="H26" s="29">
+        <v>3</v>
+      </c>
+      <c r="I26" s="30">
         <v>0</v>
       </c>
-      <c r="I26" s="31">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="J26" s="51"/>
-      <c r="K26" s="61"/>
+      <c r="J26" s="31">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="K26" s="51"/>
       <c r="L26" s="61"/>
       <c r="M26" s="61"/>
       <c r="N26" s="61"/>
@@ -4607,38 +4912,48 @@
       <c r="BL26" s="61"/>
       <c r="BM26" s="61"/>
       <c r="BN26" s="61"/>
+      <c r="BO26" s="61"/>
+      <c r="BP26" s="61"/>
+      <c r="BQ26" s="61"/>
+      <c r="BR26" s="61"/>
+      <c r="BS26" s="61"/>
+      <c r="BT26" s="61"/>
+      <c r="BU26" s="61"/>
+      <c r="BV26" s="61"/>
     </row>
-    <row r="27" spans="1:66" s="28" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:74" s="28" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="27" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.2</v>
       </c>
       <c r="B27" s="80" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="C27" s="28" t="s">
         <v>20</v>
       </c>
       <c r="D27" s="81"/>
-      <c r="E27" s="56">
-        <v>43928</v>
-      </c>
-      <c r="F27" s="57">
-        <f t="shared" si="6"/>
-        <v>43933</v>
-      </c>
-      <c r="G27" s="29">
-        <v>6</v>
-      </c>
-      <c r="H27" s="30">
+      <c r="E27" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" s="56">
+        <v>43967</v>
+      </c>
+      <c r="G27" s="57">
+        <f t="shared" si="14"/>
+        <v>43968</v>
+      </c>
+      <c r="H27" s="29">
+        <v>2</v>
+      </c>
+      <c r="I27" s="30">
         <v>0</v>
       </c>
-      <c r="I27" s="31">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="J27" s="51"/>
-      <c r="K27" s="61"/>
+      <c r="J27" s="31">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="K27" s="51"/>
       <c r="L27" s="61"/>
       <c r="M27" s="61"/>
       <c r="N27" s="61"/>
@@ -4694,38 +5009,48 @@
       <c r="BL27" s="61"/>
       <c r="BM27" s="61"/>
       <c r="BN27" s="61"/>
+      <c r="BO27" s="61"/>
+      <c r="BP27" s="61"/>
+      <c r="BQ27" s="61"/>
+      <c r="BR27" s="61"/>
+      <c r="BS27" s="61"/>
+      <c r="BT27" s="61"/>
+      <c r="BU27" s="61"/>
+      <c r="BV27" s="61"/>
     </row>
-    <row r="28" spans="1:66" s="28" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:74" s="28" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="27" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.3</v>
       </c>
       <c r="B28" s="80" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C28" s="28" t="s">
         <v>22</v>
       </c>
       <c r="D28" s="81"/>
-      <c r="E28" s="56">
-        <v>43929</v>
-      </c>
-      <c r="F28" s="57">
-        <f t="shared" si="6"/>
-        <v>43932</v>
-      </c>
-      <c r="G28" s="29">
-        <v>4</v>
-      </c>
-      <c r="H28" s="30">
+      <c r="E28" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" s="56">
+        <v>43968</v>
+      </c>
+      <c r="G28" s="57">
+        <f t="shared" si="14"/>
+        <v>43969</v>
+      </c>
+      <c r="H28" s="29">
+        <v>2</v>
+      </c>
+      <c r="I28" s="30">
         <v>0</v>
       </c>
-      <c r="I28" s="31">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="J28" s="51"/>
-      <c r="K28" s="61"/>
+      <c r="J28" s="31">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="K28" s="51"/>
       <c r="L28" s="61"/>
       <c r="M28" s="61"/>
       <c r="N28" s="61"/>
@@ -4781,38 +5106,48 @@
       <c r="BL28" s="61"/>
       <c r="BM28" s="61"/>
       <c r="BN28" s="61"/>
+      <c r="BO28" s="61"/>
+      <c r="BP28" s="61"/>
+      <c r="BQ28" s="61"/>
+      <c r="BR28" s="61"/>
+      <c r="BS28" s="61"/>
+      <c r="BT28" s="61"/>
+      <c r="BU28" s="61"/>
+      <c r="BV28" s="61"/>
     </row>
-    <row r="29" spans="1:66" s="28" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:74" s="28" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" s="27" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.4</v>
       </c>
       <c r="B29" s="80" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="C29" s="28" t="s">
         <v>24</v>
       </c>
       <c r="D29" s="81"/>
-      <c r="E29" s="56">
-        <v>43930</v>
-      </c>
-      <c r="F29" s="57">
-        <f t="shared" si="6"/>
-        <v>43934</v>
-      </c>
-      <c r="G29" s="29">
-        <v>5</v>
-      </c>
-      <c r="H29" s="30">
+      <c r="E29" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" s="56">
+        <v>43969</v>
+      </c>
+      <c r="G29" s="57">
+        <f t="shared" si="14"/>
+        <v>43970</v>
+      </c>
+      <c r="H29" s="29">
+        <v>2</v>
+      </c>
+      <c r="I29" s="30">
         <v>0</v>
       </c>
-      <c r="I29" s="31">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="J29" s="51"/>
-      <c r="K29" s="61"/>
+      <c r="J29" s="31">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
+      <c r="K29" s="51"/>
       <c r="L29" s="61"/>
       <c r="M29" s="61"/>
       <c r="N29" s="61"/>
@@ -4868,38 +5203,48 @@
       <c r="BL29" s="61"/>
       <c r="BM29" s="61"/>
       <c r="BN29" s="61"/>
+      <c r="BO29" s="61"/>
+      <c r="BP29" s="61"/>
+      <c r="BQ29" s="61"/>
+      <c r="BR29" s="61"/>
+      <c r="BS29" s="61"/>
+      <c r="BT29" s="61"/>
+      <c r="BU29" s="61"/>
+      <c r="BV29" s="61"/>
     </row>
-    <row r="30" spans="1:66" s="28" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:74" s="28" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="27" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.5</v>
       </c>
       <c r="B30" s="80" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D30" s="81"/>
-      <c r="E30" s="56">
-        <v>43931</v>
-      </c>
-      <c r="F30" s="57">
-        <f t="shared" si="6"/>
-        <v>43937</v>
-      </c>
-      <c r="G30" s="29">
-        <v>7</v>
-      </c>
-      <c r="H30" s="30">
+      <c r="E30" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F30" s="56">
+        <v>43970</v>
+      </c>
+      <c r="G30" s="57">
+        <f t="shared" si="14"/>
+        <v>43970</v>
+      </c>
+      <c r="H30" s="29">
+        <v>1</v>
+      </c>
+      <c r="I30" s="30">
         <v>0</v>
       </c>
-      <c r="I30" s="31">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="J30" s="51"/>
-      <c r="K30" s="61"/>
+      <c r="J30" s="31">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="K30" s="51"/>
       <c r="L30" s="61"/>
       <c r="M30" s="61"/>
       <c r="N30" s="61"/>
@@ -4955,27 +5300,39 @@
       <c r="BL30" s="61"/>
       <c r="BM30" s="61"/>
       <c r="BN30" s="61"/>
+      <c r="BO30" s="61"/>
+      <c r="BP30" s="61"/>
+      <c r="BQ30" s="61"/>
+      <c r="BR30" s="61"/>
+      <c r="BS30" s="61"/>
+      <c r="BT30" s="61"/>
+      <c r="BU30" s="61"/>
+      <c r="BV30" s="61"/>
     </row>
-    <row r="31" spans="1:66" s="28" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:74" s="28" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="27">
         <v>3.6</v>
       </c>
       <c r="B31" s="80" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D31" s="86"/>
-      <c r="E31" s="97"/>
-      <c r="F31" s="98"/>
-      <c r="G31" s="99"/>
-      <c r="H31" s="100">
+      <c r="E31" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F31" s="56">
+        <v>43970</v>
+      </c>
+      <c r="G31" s="89"/>
+      <c r="H31" s="90"/>
+      <c r="I31" s="91">
         <v>0</v>
       </c>
-      <c r="I31" s="101"/>
-      <c r="J31" s="102"/>
-      <c r="K31" s="61"/>
+      <c r="J31" s="92"/>
+      <c r="K31" s="93"/>
       <c r="L31" s="61"/>
       <c r="M31" s="61"/>
       <c r="N31" s="61"/>
@@ -5031,22 +5388,30 @@
       <c r="BL31" s="61"/>
       <c r="BM31" s="61"/>
       <c r="BN31" s="61"/>
+      <c r="BO31" s="61"/>
+      <c r="BP31" s="61"/>
+      <c r="BQ31" s="61"/>
+      <c r="BR31" s="61"/>
+      <c r="BS31" s="61"/>
+      <c r="BT31" s="61"/>
+      <c r="BU31" s="61"/>
+      <c r="BV31" s="61"/>
     </row>
-    <row r="32" spans="1:66" s="22" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:74" s="22" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="20">
         <v>4</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D32" s="23"/>
-      <c r="E32" s="58"/>
+      <c r="E32" s="23"/>
       <c r="F32" s="58"/>
-      <c r="G32" s="24"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="52"/>
-      <c r="K32" s="63"/>
+      <c r="G32" s="58"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="52"/>
       <c r="L32" s="63"/>
       <c r="M32" s="63"/>
       <c r="N32" s="63"/>
@@ -5102,28 +5467,36 @@
       <c r="BL32" s="63"/>
       <c r="BM32" s="63"/>
       <c r="BN32" s="63"/>
+      <c r="BO32" s="63"/>
+      <c r="BP32" s="63"/>
+      <c r="BQ32" s="63"/>
+      <c r="BR32" s="63"/>
+      <c r="BS32" s="63"/>
+      <c r="BT32" s="63"/>
+      <c r="BU32" s="63"/>
+      <c r="BV32" s="63"/>
     </row>
-    <row r="33" spans="1:66" s="28" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:67" s="28" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="27" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.1</v>
       </c>
       <c r="B33" s="80" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D33" s="81"/>
-      <c r="E33" s="56">
-        <v>43895</v>
-      </c>
-      <c r="F33" s="57"/>
-      <c r="G33" s="29"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="31"/>
-      <c r="J33" s="51"/>
-      <c r="K33" s="61"/>
+      <c r="E33" s="81"/>
+      <c r="F33" s="56">
+        <v>43905</v>
+      </c>
+      <c r="G33" s="57"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="31"/>
+      <c r="K33" s="51"/>
       <c r="L33" s="61"/>
       <c r="M33" s="61"/>
       <c r="N33" s="61"/>
@@ -5179,27 +5552,28 @@
       <c r="BL33" s="61"/>
       <c r="BM33" s="61"/>
       <c r="BN33" s="61"/>
+      <c r="BO33" s="61"/>
     </row>
-    <row r="34" spans="1:66" s="28" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:67" s="28" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="27">
         <v>4.2</v>
       </c>
       <c r="B34" s="80" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C34" s="28" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D34" s="81"/>
-      <c r="E34" s="56">
-        <v>43896</v>
-      </c>
-      <c r="F34" s="57"/>
-      <c r="G34" s="29"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="31"/>
-      <c r="J34" s="51"/>
-      <c r="K34" s="61"/>
+      <c r="E34" s="81"/>
+      <c r="F34" s="56">
+        <v>43938</v>
+      </c>
+      <c r="G34" s="57"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="31"/>
+      <c r="K34" s="51"/>
       <c r="L34" s="61"/>
       <c r="M34" s="61"/>
       <c r="N34" s="61"/>
@@ -5255,28 +5629,29 @@
       <c r="BL34" s="61"/>
       <c r="BM34" s="61"/>
       <c r="BN34" s="61"/>
+      <c r="BO34" s="61"/>
     </row>
-    <row r="35" spans="1:66" s="28" customFormat="1" ht="24" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:67" s="28" customFormat="1" ht="24" x14ac:dyDescent="0.2">
       <c r="A35" s="27" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.3</v>
       </c>
       <c r="B35" s="80" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C35" s="28" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D35" s="81"/>
-      <c r="E35" s="56">
-        <v>43897</v>
-      </c>
-      <c r="F35" s="57"/>
-      <c r="G35" s="29"/>
-      <c r="H35" s="30"/>
-      <c r="I35" s="31"/>
-      <c r="J35" s="51"/>
-      <c r="K35" s="61"/>
+      <c r="E35" s="81"/>
+      <c r="F35" s="56">
+        <v>43939</v>
+      </c>
+      <c r="G35" s="57"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="30"/>
+      <c r="J35" s="31"/>
+      <c r="K35" s="51"/>
       <c r="L35" s="61"/>
       <c r="M35" s="61"/>
       <c r="N35" s="61"/>
@@ -5332,27 +5707,28 @@
       <c r="BL35" s="61"/>
       <c r="BM35" s="61"/>
       <c r="BN35" s="61"/>
+      <c r="BO35" s="61"/>
     </row>
-    <row r="36" spans="1:66" s="28" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:67" s="28" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A36" s="27">
         <v>4.4000000000000004</v>
       </c>
       <c r="B36" s="80" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C36" s="28" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D36" s="81"/>
-      <c r="E36" s="56">
-        <v>43898</v>
-      </c>
-      <c r="F36" s="57"/>
-      <c r="G36" s="29"/>
-      <c r="H36" s="30"/>
-      <c r="I36" s="31"/>
-      <c r="J36" s="51"/>
-      <c r="K36" s="61"/>
+      <c r="E36" s="81"/>
+      <c r="F36" s="56">
+        <v>43940</v>
+      </c>
+      <c r="G36" s="57"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="30"/>
+      <c r="J36" s="31"/>
+      <c r="K36" s="51"/>
       <c r="L36" s="61"/>
       <c r="M36" s="61"/>
       <c r="N36" s="61"/>
@@ -5408,28 +5784,29 @@
       <c r="BL36" s="61"/>
       <c r="BM36" s="61"/>
       <c r="BN36" s="61"/>
+      <c r="BO36" s="61"/>
     </row>
-    <row r="37" spans="1:66" s="28" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:67" s="28" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" s="27" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.5</v>
       </c>
       <c r="B37" s="80" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C37" s="28" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D37" s="81"/>
-      <c r="E37" s="56">
-        <v>43899</v>
-      </c>
-      <c r="F37" s="57"/>
-      <c r="G37" s="29"/>
-      <c r="H37" s="30"/>
-      <c r="I37" s="31"/>
-      <c r="J37" s="51"/>
-      <c r="K37" s="61"/>
+      <c r="E37" s="81"/>
+      <c r="F37" s="56">
+        <v>43965</v>
+      </c>
+      <c r="G37" s="57"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="30"/>
+      <c r="J37" s="31"/>
+      <c r="K37" s="51"/>
       <c r="L37" s="61"/>
       <c r="M37" s="61"/>
       <c r="N37" s="61"/>
@@ -5485,22 +5862,23 @@
       <c r="BL37" s="61"/>
       <c r="BM37" s="61"/>
       <c r="BN37" s="61"/>
+      <c r="BO37" s="61"/>
     </row>
-    <row r="38" spans="1:66" s="37" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:67" s="37" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="27"/>
       <c r="B38" s="32"/>
       <c r="C38" s="32"/>
       <c r="D38" s="33"/>
-      <c r="E38" s="59"/>
+      <c r="E38" s="33"/>
       <c r="F38" s="59"/>
-      <c r="G38" s="34"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="36" t="str">
-        <f t="shared" si="4"/>
+      <c r="G38" s="59"/>
+      <c r="H38" s="34"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="36" t="str">
+        <f t="shared" si="12"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J38" s="53"/>
-      <c r="K38" s="61"/>
+      <c r="K38" s="53"/>
       <c r="L38" s="61"/>
       <c r="M38" s="61"/>
       <c r="N38" s="61"/>
@@ -5556,22 +5934,23 @@
       <c r="BL38" s="61"/>
       <c r="BM38" s="61"/>
       <c r="BN38" s="61"/>
+      <c r="BO38" s="61"/>
     </row>
-    <row r="39" spans="1:66" s="37" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:67" s="37" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" s="27"/>
       <c r="B39" s="32"/>
       <c r="C39" s="32"/>
       <c r="D39" s="33"/>
-      <c r="E39" s="59"/>
+      <c r="E39" s="33"/>
       <c r="F39" s="59"/>
-      <c r="G39" s="34"/>
-      <c r="H39" s="35"/>
-      <c r="I39" s="36" t="str">
-        <f t="shared" si="4"/>
+      <c r="G39" s="59"/>
+      <c r="H39" s="34"/>
+      <c r="I39" s="35"/>
+      <c r="J39" s="36" t="str">
+        <f t="shared" si="12"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J39" s="53"/>
-      <c r="K39" s="61"/>
+      <c r="K39" s="53"/>
       <c r="L39" s="61"/>
       <c r="M39" s="61"/>
       <c r="N39" s="61"/>
@@ -5627,10 +6006,10 @@
       <c r="BL39" s="61"/>
       <c r="BM39" s="61"/>
       <c r="BN39" s="61"/>
+      <c r="BO39" s="61"/>
     </row>
-    <row r="40" spans="1:66" s="38" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="J40" s="54"/>
-      <c r="K40" s="61"/>
+    <row r="40" spans="1:67" s="38" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="K40" s="54"/>
       <c r="L40" s="61"/>
       <c r="M40" s="61"/>
       <c r="N40" s="61"/>
@@ -5686,10 +6065,10 @@
       <c r="BL40" s="61"/>
       <c r="BM40" s="61"/>
       <c r="BN40" s="61"/>
+      <c r="BO40" s="61"/>
     </row>
-    <row r="41" spans="1:66" s="37" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="J41" s="54"/>
-      <c r="K41" s="61"/>
+    <row r="41" spans="1:67" s="37" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="K41" s="54"/>
       <c r="L41" s="61"/>
       <c r="M41" s="61"/>
       <c r="N41" s="61"/>
@@ -5745,10 +6124,10 @@
       <c r="BL41" s="61"/>
       <c r="BM41" s="61"/>
       <c r="BN41" s="61"/>
+      <c r="BO41" s="61"/>
     </row>
-    <row r="42" spans="1:66" s="37" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="J42" s="55"/>
-      <c r="K42" s="61"/>
+    <row r="42" spans="1:67" s="37" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="K42" s="55"/>
       <c r="L42" s="61"/>
       <c r="M42" s="61"/>
       <c r="N42" s="61"/>
@@ -5804,8 +6183,9 @@
       <c r="BL42" s="61"/>
       <c r="BM42" s="61"/>
       <c r="BN42" s="61"/>
+      <c r="BO42" s="61"/>
     </row>
-    <row r="43" spans="1:66" s="37" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:67" s="37" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -5815,8 +6195,8 @@
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
       <c r="I43" s="7"/>
-      <c r="J43" s="55"/>
-      <c r="K43" s="61"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="55"/>
       <c r="L43" s="61"/>
       <c r="M43" s="61"/>
       <c r="N43" s="61"/>
@@ -5872,8 +6252,9 @@
       <c r="BL43" s="61"/>
       <c r="BM43" s="61"/>
       <c r="BN43" s="61"/>
+      <c r="BO43" s="61"/>
     </row>
-    <row r="44" spans="1:66" s="37" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:67" s="37" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -5883,8 +6264,8 @@
       <c r="G44" s="7"/>
       <c r="H44" s="7"/>
       <c r="I44" s="7"/>
-      <c r="J44" s="55"/>
-      <c r="K44" s="61"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="55"/>
       <c r="L44" s="61"/>
       <c r="M44" s="61"/>
       <c r="N44" s="61"/>
@@ -5940,25 +6321,26 @@
       <c r="BL44" s="61"/>
       <c r="BM44" s="61"/>
       <c r="BN44" s="61"/>
+      <c r="BO44" s="61"/>
     </row>
-    <row r="45" spans="1:66" s="37" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:67" s="37" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
       <c r="D45" s="87"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7" t="str">
-        <f t="shared" ref="F45:F47" si="9">IF(ISBLANK(E45)," - ",IF(G45=0,E45,E45+G45-1))</f>
+      <c r="E45" s="87"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7" t="str">
+        <f t="shared" ref="G45:G47" si="17">IF(ISBLANK(F45)," - ",IF(H45=0,F45,F45+H45-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="G45" s="7"/>
       <c r="H45" s="7"/>
-      <c r="I45" s="7" t="str">
-        <f>IF(OR(F45=0,E45=0)," - ",NETWORKDAYS(E45,F45))</f>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7" t="str">
+        <f>IF(OR(G45=0,F45=0)," - ",NETWORKDAYS(F45,G45))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J45" s="55"/>
-      <c r="K45" s="61"/>
+      <c r="K45" s="55"/>
       <c r="L45" s="61"/>
       <c r="M45" s="61"/>
       <c r="N45" s="61"/>
@@ -6014,24 +6396,25 @@
       <c r="BL45" s="61"/>
       <c r="BM45" s="61"/>
       <c r="BN45" s="61"/>
+      <c r="BO45" s="61"/>
     </row>
-    <row r="46" spans="1:66" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:67" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
       <c r="D46" s="87"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7" t="str">
-        <f t="shared" si="9"/>
+      <c r="E46" s="87"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7" t="str">
+        <f t="shared" si="17"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="G46" s="7"/>
       <c r="H46" s="7"/>
-      <c r="I46" s="7" t="str">
-        <f t="shared" ref="I46:I48" si="10">IF(OR(F46=0,E46=0)," - ",NETWORKDAYS(E46,F46))</f>
+      <c r="I46" s="7"/>
+      <c r="J46" s="7" t="str">
+        <f t="shared" ref="J46:J48" si="18">IF(OR(G46=0,F46=0)," - ",NETWORKDAYS(F46,G46))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J46" s="10"/>
       <c r="K46" s="10"/>
       <c r="L46" s="10"/>
       <c r="M46" s="10"/>
@@ -6088,77 +6471,83 @@
       <c r="BL46" s="10"/>
       <c r="BM46" s="10"/>
       <c r="BN46" s="10"/>
+      <c r="BO46" s="10"/>
     </row>
-    <row r="47" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47" s="87"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7" t="str">
-        <f t="shared" si="9"/>
+      <c r="E47" s="87"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7" t="str">
+        <f t="shared" si="17"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="G47" s="7"/>
       <c r="H47" s="7"/>
-      <c r="I47" s="7" t="str">
-        <f t="shared" si="10"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7" t="str">
+        <f t="shared" si="18"/>
         <v xml:space="preserve"> - </v>
       </c>
     </row>
-    <row r="48" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="87"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7" t="str">
-        <f>IF(ISBLANK(E48)," - ",IF(#REF!=0,E48,E48+#REF!-1))</f>
+      <c r="E48" s="87"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7" t="str">
+        <f>IF(ISBLANK(F48)," - ",IF(#REF!=0,F48,F48+#REF!-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="G48" s="7"/>
       <c r="H48" s="7"/>
-      <c r="I48" s="7" t="str">
-        <f t="shared" si="10"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="7" t="str">
+        <f t="shared" si="18"/>
         <v xml:space="preserve"> - </v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="85"/>
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
       <c r="D49" s="11"/>
-      <c r="E49" s="10"/>
+      <c r="E49" s="11"/>
       <c r="F49" s="10"/>
       <c r="G49" s="10"/>
       <c r="H49" s="10"/>
       <c r="I49" s="10"/>
+      <c r="J49" s="10"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
-  <mergeCells count="19">
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
-    <mergeCell ref="AF4:AL4"/>
-    <mergeCell ref="AF5:AL5"/>
-    <mergeCell ref="BH4:BN4"/>
-    <mergeCell ref="BH5:BN5"/>
-    <mergeCell ref="AM5:AS5"/>
-    <mergeCell ref="AT4:AZ4"/>
-    <mergeCell ref="AT5:AZ5"/>
-    <mergeCell ref="AM4:AS4"/>
-    <mergeCell ref="BA4:BG4"/>
-    <mergeCell ref="BA5:BG5"/>
+  <mergeCells count="21">
+    <mergeCell ref="BP5:BV5"/>
+    <mergeCell ref="BP4:BV4"/>
+    <mergeCell ref="AG4:AM4"/>
+    <mergeCell ref="AG5:AM5"/>
+    <mergeCell ref="BI4:BO4"/>
+    <mergeCell ref="BI5:BO5"/>
+    <mergeCell ref="AN5:AT5"/>
+    <mergeCell ref="AU4:BA4"/>
+    <mergeCell ref="AU5:BA5"/>
+    <mergeCell ref="AN4:AT4"/>
+    <mergeCell ref="BB4:BH4"/>
+    <mergeCell ref="BB5:BH5"/>
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="H43:H48 H8:H39">
+  <conditionalFormatting sqref="I43:I48 I8:I39">
     <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -6172,44 +6561,52 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K6:BN7">
-    <cfRule type="expression" dxfId="5" priority="45">
-      <formula>K$6=TODAY()</formula>
+  <conditionalFormatting sqref="L6:BV7">
+    <cfRule type="expression" dxfId="7" priority="45">
+      <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K8:BN39">
-    <cfRule type="expression" dxfId="4" priority="48">
-      <formula>AND($E8&lt;=K$6,ROUNDDOWN(($F8-$E8+1)*$H8,0)+$E8-1&gt;=K$6)</formula>
+  <conditionalFormatting sqref="L8:BV13 L15:BV19 L20:BO39 BP20:BV32">
+    <cfRule type="expression" dxfId="6" priority="48">
+      <formula>AND($F8&lt;=L$6,ROUNDDOWN(($G8-$F8+1)*$I8,0)+$F8-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="49">
-      <formula>AND(NOT(ISBLANK($E8)),$E8&lt;=K$6,$F8&gt;=K$6)</formula>
+    <cfRule type="expression" dxfId="5" priority="49">
+      <formula>AND(NOT(ISBLANK($F8)),$F8&lt;=L$6,$G8&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K6:BN45">
-    <cfRule type="expression" dxfId="2" priority="8">
-      <formula>K$6=TODAY()</formula>
+  <conditionalFormatting sqref="BW6:DS7 L6:BO45 BP6:BV32">
+    <cfRule type="expression" dxfId="4" priority="8">
+      <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K40:BN45">
-    <cfRule type="expression" dxfId="1" priority="55">
-      <formula>AND($E43&lt;=K$6,ROUNDDOWN(($F43-$E43+1)*$H43,0)+$E43-1&gt;=K$6)</formula>
+  <conditionalFormatting sqref="L40:BO45">
+    <cfRule type="expression" dxfId="3" priority="55">
+      <formula>AND($F43&lt;=L$6,ROUNDDOWN(($G43-$F43+1)*$I43,0)+$F43-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="56">
-      <formula>AND(NOT(ISBLANK($E43)),$E43&lt;=K$6,$F43&gt;=K$6)</formula>
+    <cfRule type="expression" dxfId="2" priority="56">
+      <formula>AND(NOT(ISBLANK($F43)),$F43&lt;=L$6,$G43&gt;=L$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L14:BV14">
+    <cfRule type="expression" dxfId="1" priority="63">
+      <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="64">
+      <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Enter the week number to display first in the Gantt Chart. The weeks are numbered starting from the week containing the Project Start Date." sqref="H4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Enter the week number to display first in the Gantt Chart. The weeks are numbered starting from the week containing the Project Start Date." sqref="I4"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="K1:AE1" r:id="rId1" display="Gantt Chart Template © 2006-2018 by Vertex42.com."/>
+    <hyperlink ref="L1:AF1" r:id="rId1" display="Gantt Chart Template © 2006-2018 by Vertex42.com."/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.5" footer="0.25"/>
   <pageSetup scale="63" fitToHeight="0" orientation="landscape" r:id="rId2"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="A38:B39 E16 E25 E38:H39 G11 G10 G16:H16 G25:H25 H20 H18 H19 H26:H29" unlockedFormula="1"/>
-    <ignoredError sqref="A25 A16" formula="1"/>
+    <ignoredError sqref="A38:B39 F17 F25 F38:I39 H11 H10 H17:I17 H25:I25 I26:I29" unlockedFormula="1"/>
+    <ignoredError sqref="A25 A17" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId3"/>
   <legacyDrawing r:id="rId4"/>
@@ -6222,13 +6619,13 @@
               <controlPr defaultSize="0" print="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>9</xdr:col>
+                    <xdr:col>10</xdr:col>
                     <xdr:colOff>95250</xdr:colOff>
                     <xdr:row>1</xdr:row>
                     <xdr:rowOff>123825</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>27</xdr:col>
+                    <xdr:col>28</xdr:col>
                     <xdr:colOff>114300</xdr:colOff>
                     <xdr:row>2</xdr:row>
                     <xdr:rowOff>114300</xdr:rowOff>
@@ -6257,7 +6654,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H43:H48 H8:H39</xm:sqref>
+          <xm:sqref>I43:I48 I8:I39</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>